<commit_message>
small change to jp spreadsheet
</commit_message>
<xml_diff>
--- a/2024-25 MDE Ed-Fi Documentation/Joint_Powers_Vendor_Certification_Pattern_Data.xlsx
+++ b/2024-25 MDE Ed-Fi Documentation/Joint_Powers_Vendor_Certification_Pattern_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDolbow\.vscode\MDE-EdFi-Documentation\2024-25 MDE Ed-Fi Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5135DB7D-2D01-46EE-8843-16DF54955D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6240B168-A560-421C-9E86-5D3C342BCB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B57C0786-A6AB-4FD4-B2B0-BA31B16F8519}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B57C0786-A6AB-4FD4-B2B0-BA31B16F8519}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -982,6 +982,60 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
     <dxf>
@@ -1200,6 +1254,60 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
     <dxf>
@@ -1306,114 +1414,6 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -4748,52 +4748,52 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{5692A297-79BF-4F9C-9126-9341754B759A}" name="SEORAs22" displayName="SEORAs22" ref="A24:G28" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{5692A297-79BF-4F9C-9126-9341754B759A}" name="SEORAs22" displayName="SEORAs22" ref="A24:G28" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A24:G28" xr:uid="{77FAAC26-2EEA-45D3-832C-0FF7AB0115F4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:G28">
     <sortCondition ref="A25:A28"/>
     <sortCondition ref="E25:E28"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{97BBDAA1-EEF4-4890-8CC6-F82A47B30DC3}" name="Student" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{E5BB4BAA-D5FE-494C-A12E-4E5CD1FEFE9B}" name="EdOrgReference SchoolID" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{A74DDED4-B75E-4848-97D9-1694DFE7B6C8}" name="StudentUniqueId" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{355E7FFD-F72E-4F56-BD11-829342E8EDCE}" name="ReportingEdOrgReference SchoolID" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{4EA8EC2D-F4E8-4AC9-8F4E-F658A2E86566}" name="BeginDate" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{6F2CC1BA-FBD7-4B28-A91B-22431AA0A9BC}" name="EndDate" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{5D24870A-BBBB-49F7-A22D-9BC354C82EE7}" name="ResponsibiltyDescriptor" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{97BBDAA1-EEF4-4890-8CC6-F82A47B30DC3}" name="Student" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{E5BB4BAA-D5FE-494C-A12E-4E5CD1FEFE9B}" name="EdOrgReference SchoolID" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{A74DDED4-B75E-4848-97D9-1694DFE7B6C8}" name="StudentUniqueId" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{355E7FFD-F72E-4F56-BD11-829342E8EDCE}" name="ReportingEdOrgReference SchoolID" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{4EA8EC2D-F4E8-4AC9-8F4E-F658A2E86566}" name="BeginDate" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{6F2CC1BA-FBD7-4B28-A91B-22431AA0A9BC}" name="EndDate" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{5D24870A-BBBB-49F7-A22D-9BC354C82EE7}" name="ResponsibiltyDescriptor" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{E2C8E32D-19BD-4526-BD62-D5BCA10CC455}" name="EdOrgIds23" displayName="EdOrgIds23" ref="D5:G10" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{E2C8E32D-19BD-4526-BD62-D5BCA10CC455}" name="EdOrgIds23" displayName="EdOrgIds23" ref="D5:G10" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="D5:G10" xr:uid="{E2C8E32D-19BD-4526-BD62-D5BCA10CC455}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FDD8D5C6-800F-4420-AE64-B80892DD5760}" name="Element" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{6E125EEB-7097-4769-8F32-19E6038EE69E}" name="Example ID" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{0922D666-F3DB-47C1-914F-77976F17A1B8}" name="Used In…For this Pattern" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{A977DE9F-420B-4361-B08C-A9FD32195551}" name="Reason" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{FDD8D5C6-800F-4420-AE64-B80892DD5760}" name="Element" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{6E125EEB-7097-4769-8F32-19E6038EE69E}" name="Example ID" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{0922D666-F3DB-47C1-914F-77976F17A1B8}" name="Used In…For this Pattern" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{A977DE9F-420B-4361-B08C-A9FD32195551}" name="Reason" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{8ECA3C70-6EF7-49D0-B684-3D141180DADB}" name="SSEPAs21" displayName="SSEPAs21" ref="A47:J51" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{8ECA3C70-6EF7-49D0-B684-3D141180DADB}" name="SSEPAs21" displayName="SSEPAs21" ref="A47:J51" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A47:J51" xr:uid="{D3CF0901-CC20-4EC6-A4BB-C588254B263D}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{E4DF4947-C3A2-484F-9044-02FFEC2121CC}" name="Student" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{7BAF099E-F389-4EF3-9391-CDA5FEC272D3}" name="EdOrgReference SchoolID" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{01FD7A9A-A19F-48A9-A931-041143D4B550}" name="StudentUniqueId" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{C5888552-F872-4891-82A6-71B6CEFFD6B1}" name="ProgramType" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{2B79307A-550E-4F01-8DD5-FE20AEC09EEF}" name="BeginDate" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{E3D74796-9820-4448-BF45-3877BF979345}" name="EndDate" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{20C673CA-FDFD-4929-A3EA-443A5768000E}" name="DisabilityDescriptor" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{B744BD5D-2FFC-4E93-9A56-B726A607287B}" name="OrderOfDisability" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{CA31B897-F85C-44E1-8EEE-B20CF3FE1A71}" name="SpecialEducationSetting" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{ACB63A65-6385-4A6E-BD2B-697EE91120C2}" name="SpecialEducationServiceHours" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{E4DF4947-C3A2-484F-9044-02FFEC2121CC}" name="Student" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{7BAF099E-F389-4EF3-9391-CDA5FEC272D3}" name="EdOrgReference SchoolID" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{01FD7A9A-A19F-48A9-A931-041143D4B550}" name="StudentUniqueId" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C5888552-F872-4891-82A6-71B6CEFFD6B1}" name="ProgramType" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{2B79307A-550E-4F01-8DD5-FE20AEC09EEF}" name="BeginDate" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{E3D74796-9820-4448-BF45-3877BF979345}" name="EndDate" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{20C673CA-FDFD-4929-A3EA-443A5768000E}" name="DisabilityDescriptor" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{B744BD5D-2FFC-4E93-9A56-B726A607287B}" name="OrderOfDisability" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{CA31B897-F85C-44E1-8EEE-B20CF3FE1A71}" name="SpecialEducationSetting" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{ACB63A65-6385-4A6E-BD2B-697EE91120C2}" name="SpecialEducationServiceHours" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5544,8 +5544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136FD443-4433-4AA8-9391-F8565D648BB7}">
   <dimension ref="A1:W96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:G42"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7244,10 +7244,10 @@
         <v>45449</v>
       </c>
       <c r="G67" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7270,10 +7270,10 @@
         <v>45216</v>
       </c>
       <c r="G68" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7296,10 +7296,10 @@
         <v>45436</v>
       </c>
       <c r="G69" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates to joint powers scenarios to make membership & attendance more consistent with typical SSAs
</commit_message>
<xml_diff>
--- a/2024-25 MDE Ed-Fi Documentation/Joint_Powers_Vendor_Certification_Pattern_Data.xlsx
+++ b/2024-25 MDE Ed-Fi Documentation/Joint_Powers_Vendor_Certification_Pattern_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDolbow\.vscode\MDE-EdFi-Documentation\2024-25 MDE Ed-Fi Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6240B168-A560-421C-9E86-5D3C342BCB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AD47F1-EDF7-46BA-95FE-7513F152BD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B57C0786-A6AB-4FD4-B2B0-BA31B16F8519}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B57C0786-A6AB-4FD4-B2B0-BA31B16F8519}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -37,44 +37,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={53C709BC-7C1F-4D55-A8EB-3519CF26184E}</author>
-  </authors>
-  <commentList>
-    <comment ref="P21" authorId="0" shapeId="0" xr:uid="{53C709BC-7C1F-4D55-A8EB-3519CF26184E}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Are we really only dealing in days for membership and attendance?</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={BFCB5ABF-48BF-4194-8828-6EA40B2FEB51}</author>
-  </authors>
-  <commentList>
-    <comment ref="P17" authorId="0" shapeId="0" xr:uid="{BFCB5ABF-48BF-4194-8828-6EA40B2FEB51}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Are we really only dealing in days for membership and attendance?</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="177">
   <si>
     <t>Tab Name</t>
   </si>
@@ -277,12 +241,6 @@
     <t>ResidentLEAReference</t>
   </si>
   <si>
-    <t>MembershipDays</t>
-  </si>
-  <si>
-    <t>AttendanceDays</t>
-  </si>
-  <si>
     <t>PercentEnrolled</t>
   </si>
   <si>
@@ -296,9 +254,6 @@
   </si>
   <si>
     <t>CalendarReference</t>
-  </si>
-  <si>
-    <t>See EE record</t>
   </si>
   <si>
     <t>EE</t>
@@ -764,8 +719,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -911,7 +867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -941,12 +897,218 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="201">
+  <dxfs count="203">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1414,42 +1576,6 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -1895,42 +2021,6 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -3292,42 +3382,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
     <dxf>
@@ -3757,60 +3811,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -4584,364 +4584,364 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Dolbow, Mike (He/Him/His) (MNIT)" id="{64E8492C-03DE-4998-8505-BC99EAD32963}" userId="S::Mike.Dolbow@state.mn.us::5fe21be2-7940-48b6-9a82-7b6131516358" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74EE680D-9ECA-44B1-A8B0-0CA4D774A219}" name="Table1" displayName="Table1" ref="A17:F21" totalsRowShown="0" headerRowDxfId="200" dataDxfId="199">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74EE680D-9ECA-44B1-A8B0-0CA4D774A219}" name="Table1" displayName="Table1" ref="A17:F21" totalsRowShown="0" headerRowDxfId="202" dataDxfId="201">
   <autoFilter ref="A17:F21" xr:uid="{74EE680D-9ECA-44B1-A8B0-0CA4D774A219}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:F21">
     <sortCondition ref="A17:A21"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="6" xr3:uid="{F244D1BA-4C44-4421-B60A-E68EB5578920}" name="Number" dataDxfId="198"/>
-    <tableColumn id="1" xr3:uid="{E6F287A9-697B-46ED-9E9F-CFD1DEC407FD}" name="Tab Name" dataDxfId="197"/>
-    <tableColumn id="5" xr3:uid="{AC5D42B3-C265-479E-BFC5-18C3F6DBC907}" name="Data Flow Direction" dataDxfId="196"/>
-    <tableColumn id="2" xr3:uid="{4B4D9704-5DE1-4530-BC82-1CBF7FBA24B7}" name="If MARSS Process Today" dataDxfId="195"/>
-    <tableColumn id="3" xr3:uid="{F768796C-F4FC-4151-AC25-66E35E1FD8BE}" name="Then Do this in EdFi" dataDxfId="194"/>
-    <tableColumn id="4" xr3:uid="{0A9A38E0-A962-4E33-8406-A760BA0775DB}" name="Notes" dataDxfId="193"/>
+    <tableColumn id="6" xr3:uid="{F244D1BA-4C44-4421-B60A-E68EB5578920}" name="Number" dataDxfId="200"/>
+    <tableColumn id="1" xr3:uid="{E6F287A9-697B-46ED-9E9F-CFD1DEC407FD}" name="Tab Name" dataDxfId="199"/>
+    <tableColumn id="5" xr3:uid="{AC5D42B3-C265-479E-BFC5-18C3F6DBC907}" name="Data Flow Direction" dataDxfId="198"/>
+    <tableColumn id="2" xr3:uid="{4B4D9704-5DE1-4530-BC82-1CBF7FBA24B7}" name="If MARSS Process Today" dataDxfId="197"/>
+    <tableColumn id="3" xr3:uid="{F768796C-F4FC-4151-AC25-66E35E1FD8BE}" name="Then Do this in EdFi" dataDxfId="196"/>
+    <tableColumn id="4" xr3:uid="{0A9A38E0-A962-4E33-8406-A760BA0775DB}" name="Notes" dataDxfId="195"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3CF0901-CC20-4EC6-A4BB-C588254B263D}" name="SSEPAs" displayName="SSEPAs" ref="A74:K80" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3CF0901-CC20-4EC6-A4BB-C588254B263D}" name="SSEPAs" displayName="SSEPAs" ref="A74:K80" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
   <autoFilter ref="A74:K80" xr:uid="{D3CF0901-CC20-4EC6-A4BB-C588254B263D}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EB40C147-90DE-48B5-8796-49E623DC4E7C}" name="Student" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{DBBEE278-F072-4B56-A6F8-DACC2223D596}" name="EdOrgReference SchoolID" dataDxfId="102"/>
-    <tableColumn id="3" xr3:uid="{C0A1BF68-1FB1-4480-B1C8-72DC3BFCAD22}" name="StudentUniqueId" dataDxfId="101"/>
-    <tableColumn id="4" xr3:uid="{24A13DCF-85C7-4DE6-8C3B-392BB7EC4C10}" name="ProgramType" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{D4EDE21F-3739-4CB6-BF74-3DFC09DC6F98}" name="BeginDate" dataDxfId="99"/>
-    <tableColumn id="6" xr3:uid="{6E1E1FFB-5065-4047-B6CE-377B73DA72C6}" name="EndDate" dataDxfId="98"/>
-    <tableColumn id="7" xr3:uid="{77B58A17-99F8-4B22-8571-A4BDF0118246}" name="DisabilityDescriptor" dataDxfId="97"/>
-    <tableColumn id="8" xr3:uid="{BC11DEE3-57F6-4A9E-B7B0-3C449D912E87}" name="OrderOfDisability" dataDxfId="96"/>
-    <tableColumn id="9" xr3:uid="{5D20C335-1671-4B9C-9E6C-CC5949CCA43E}" name="SpecialEducationSetting" dataDxfId="95"/>
-    <tableColumn id="10" xr3:uid="{4F4D10F4-5E8F-4AB4-81B1-7AB2D9F3AB81}" name="SpecialEducationServiceHours" dataDxfId="94"/>
-    <tableColumn id="11" xr3:uid="{D96C9E4B-D2F3-4C15-81D1-FA31E1D96253}" name="Notes" dataDxfId="93"/>
+    <tableColumn id="1" xr3:uid="{EB40C147-90DE-48B5-8796-49E623DC4E7C}" name="Student" dataDxfId="110"/>
+    <tableColumn id="2" xr3:uid="{DBBEE278-F072-4B56-A6F8-DACC2223D596}" name="EdOrgReference SchoolID" dataDxfId="109"/>
+    <tableColumn id="3" xr3:uid="{C0A1BF68-1FB1-4480-B1C8-72DC3BFCAD22}" name="StudentUniqueId" dataDxfId="108"/>
+    <tableColumn id="4" xr3:uid="{24A13DCF-85C7-4DE6-8C3B-392BB7EC4C10}" name="ProgramType" dataDxfId="107"/>
+    <tableColumn id="5" xr3:uid="{D4EDE21F-3739-4CB6-BF74-3DFC09DC6F98}" name="BeginDate" dataDxfId="106"/>
+    <tableColumn id="6" xr3:uid="{6E1E1FFB-5065-4047-B6CE-377B73DA72C6}" name="EndDate" dataDxfId="105"/>
+    <tableColumn id="7" xr3:uid="{77B58A17-99F8-4B22-8571-A4BDF0118246}" name="DisabilityDescriptor" dataDxfId="104"/>
+    <tableColumn id="8" xr3:uid="{BC11DEE3-57F6-4A9E-B7B0-3C449D912E87}" name="OrderOfDisability" dataDxfId="103"/>
+    <tableColumn id="9" xr3:uid="{5D20C335-1671-4B9C-9E6C-CC5949CCA43E}" name="SpecialEducationSetting" dataDxfId="102"/>
+    <tableColumn id="10" xr3:uid="{4F4D10F4-5E8F-4AB4-81B1-7AB2D9F3AB81}" name="SpecialEducationServiceHours" dataDxfId="101"/>
+    <tableColumn id="11" xr3:uid="{D96C9E4B-D2F3-4C15-81D1-FA31E1D96253}" name="Notes" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{77FAAC26-2EEA-45D3-832C-0FF7AB0115F4}" name="SEORAs" displayName="SEORAs" ref="A33:G42" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{77FAAC26-2EEA-45D3-832C-0FF7AB0115F4}" name="SEORAs" displayName="SEORAs" ref="A33:G42" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
   <autoFilter ref="A33:G42" xr:uid="{77FAAC26-2EEA-45D3-832C-0FF7AB0115F4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:G42">
     <sortCondition ref="A34:A42"/>
     <sortCondition ref="E34:E42"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F05BB232-4DFB-4C6E-811E-2AF6253132F7}" name="Student" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{D4736AE3-CC59-41EA-BFA9-4EDC5622C627}" name="EdOrgReference SchoolID" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{344E6356-7C86-47AB-A9B5-171414F3EFAC}" name="StudentUniqueId" dataDxfId="88"/>
-    <tableColumn id="4" xr3:uid="{83C6D33C-247C-40CF-8422-32BAE1ACE4BA}" name="ReportingEdOrgReference SchoolID" dataDxfId="87"/>
-    <tableColumn id="5" xr3:uid="{16307EDC-78DB-420B-8467-0BAD8C2391FD}" name="BeginDate" dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{2B61E709-93D0-41FC-BD9F-DA062C218CAC}" name="EndDate" dataDxfId="85"/>
-    <tableColumn id="7" xr3:uid="{46451781-17EF-44AB-BF2B-B4E3194F2583}" name="ResponsibiltyDescriptor" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{F05BB232-4DFB-4C6E-811E-2AF6253132F7}" name="Student" dataDxfId="97"/>
+    <tableColumn id="2" xr3:uid="{D4736AE3-CC59-41EA-BFA9-4EDC5622C627}" name="EdOrgReference SchoolID" dataDxfId="96"/>
+    <tableColumn id="3" xr3:uid="{344E6356-7C86-47AB-A9B5-171414F3EFAC}" name="StudentUniqueId" dataDxfId="95"/>
+    <tableColumn id="4" xr3:uid="{83C6D33C-247C-40CF-8422-32BAE1ACE4BA}" name="ReportingEdOrgReference SchoolID" dataDxfId="94"/>
+    <tableColumn id="5" xr3:uid="{16307EDC-78DB-420B-8467-0BAD8C2391FD}" name="BeginDate" dataDxfId="93"/>
+    <tableColumn id="6" xr3:uid="{2B61E709-93D0-41FC-BD9F-DA062C218CAC}" name="EndDate" dataDxfId="92"/>
+    <tableColumn id="7" xr3:uid="{46451781-17EF-44AB-BF2B-B4E3194F2583}" name="ResponsibiltyDescriptor" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{7A4D8A4E-B4D6-48EF-AE93-C41CB990E854}" name="Students13" displayName="Students13" ref="A5:B7" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{7A4D8A4E-B4D6-48EF-AE93-C41CB990E854}" name="Students13" displayName="Students13" ref="A5:B7" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
   <autoFilter ref="A5:B7" xr:uid="{E813628D-9E65-466B-AFAE-06C8ED720622}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{299B3E39-4326-4464-A557-F9C8B0EAC6B3}" name="Generic Name" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{062A82B9-5087-4506-AA8E-D7FE1B7660B4}" name="ID" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{299B3E39-4326-4464-A557-F9C8B0EAC6B3}" name="Generic Name" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{062A82B9-5087-4506-AA8E-D7FE1B7660B4}" name="ID" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{EE1C7247-5C59-4215-B4C5-0E8837A2BAF6}" name="Scenarios14" displayName="Scenarios14" ref="A12:C14" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{EE1C7247-5C59-4215-B4C5-0E8837A2BAF6}" name="Scenarios14" displayName="Scenarios14" ref="A12:C14" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
   <autoFilter ref="A12:C14" xr:uid="{6D6F743E-9CB8-4440-92A1-95FD6FFE6308}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{13C3256E-0CEE-41E5-85AC-724669B68AA2}" name="Scenario Identifier" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{F64DDA22-2EF1-4AB5-954C-9266230EF577}" name="Student" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{68C9BC3C-2995-4DCA-9514-BD8AA004ECC9}" name="Description" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{13C3256E-0CEE-41E5-85AC-724669B68AA2}" name="Scenario Identifier" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{F64DDA22-2EF1-4AB5-954C-9266230EF577}" name="Student" dataDxfId="83"/>
+    <tableColumn id="2" xr3:uid="{68C9BC3C-2995-4DCA-9514-BD8AA004ECC9}" name="Description" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{2C1A36F6-A443-478F-8632-701D4AC088EF}" name="SSAs15" displayName="SSAs15" ref="A17:T21" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
-  <autoFilter ref="A17:T21" xr:uid="{85C15CF2-370D-42B8-85DC-039C7BB0A730}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:T21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{2C1A36F6-A443-478F-8632-701D4AC088EF}" name="SSAs15" displayName="SSAs15" ref="A17:U21" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+  <autoFilter ref="A17:U21" xr:uid="{85C15CF2-370D-42B8-85DC-039C7BB0A730}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:U21">
     <sortCondition ref="A18:A21"/>
     <sortCondition ref="E18:E21"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{77BD5FE2-7D29-4278-B63A-7A06AF887945}" name="Student" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{490DFC55-A99B-4943-BC4F-82BC3BAE0AB2}" name="SchoolYear" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{379DFE0A-3603-4E83-A069-1909CEEF2FBB}" name="SchoolReference SchoolID" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{954AA04A-3355-4EA1-8BF8-8B54D100FDED}" name="StudentUniqueId" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{9D720E08-5DCB-4550-8EC5-5DB73369328B}" name="EntryDate" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{248E7E85-0636-44F6-A9B7-3822FE17505C}" name="EntryType" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{8AB87614-E268-4037-B124-AD289B2038D3}" name="EntryGradeLevel" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{1E0CAC48-E2F8-4439-9A70-142378B29E11}" name="ExitWithdrawDate" dataDxfId="65"/>
-    <tableColumn id="9" xr3:uid="{8E363293-A545-4028-86AB-56D402E6B5DF}" name="ExitWithdrawType" dataDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{643BDE56-57B7-44F0-9BF5-CBB7C61DE871}" name="CalendarReference" dataDxfId="63"/>
-    <tableColumn id="11" xr3:uid="{EA285CC7-0C07-4807-BAE0-C470FB431A3C}" name="SpecialEdEvalStatus" dataDxfId="62"/>
-    <tableColumn id="12" xr3:uid="{E4A73A11-17B0-47E2-9CA5-C2E7F1C386F4}" name="StateAidCategory" dataDxfId="61"/>
-    <tableColumn id="13" xr3:uid="{9479A754-4670-458F-9436-083720FA4EBA}" name="HomeboundService" dataDxfId="60"/>
-    <tableColumn id="14" xr3:uid="{C3053064-2B1E-4443-9801-38762BA25785}" name="SpecialPupil" dataDxfId="59"/>
-    <tableColumn id="15" xr3:uid="{6901B54C-5DCF-4EAB-9F58-2FE573BC7343}" name="ResidentLEAReference" dataDxfId="58"/>
-    <tableColumn id="16" xr3:uid="{303CB387-33E4-4656-9582-02D45831B388}" name="AttendanceDays" dataDxfId="57"/>
-    <tableColumn id="17" xr3:uid="{0705E415-91EB-4AF5-A47D-97AE74014A06}" name="MembershipDays" dataDxfId="56"/>
-    <tableColumn id="18" xr3:uid="{9846E1C6-D5CD-422C-B9CF-54925AEC931C}" name="PercentEnrolled" dataDxfId="55"/>
-    <tableColumn id="19" xr3:uid="{7730A9C1-1558-4B94-AD1E-5AC7983CABDF}" name="TransportationCategory" dataDxfId="54"/>
-    <tableColumn id="20" xr3:uid="{0E474587-197B-49DB-A30A-C0D1EA91022A}" name="TransportationLEA" dataDxfId="53"/>
+  <tableColumns count="21">
+    <tableColumn id="1" xr3:uid="{77BD5FE2-7D29-4278-B63A-7A06AF887945}" name="Student" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{490DFC55-A99B-4943-BC4F-82BC3BAE0AB2}" name="SchoolYear" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{379DFE0A-3603-4E83-A069-1909CEEF2FBB}" name="SchoolReference SchoolID" dataDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{954AA04A-3355-4EA1-8BF8-8B54D100FDED}" name="StudentUniqueId" dataDxfId="76"/>
+    <tableColumn id="5" xr3:uid="{9D720E08-5DCB-4550-8EC5-5DB73369328B}" name="EntryDate" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{248E7E85-0636-44F6-A9B7-3822FE17505C}" name="EntryType" dataDxfId="74"/>
+    <tableColumn id="7" xr3:uid="{8AB87614-E268-4037-B124-AD289B2038D3}" name="EntryGradeLevel" dataDxfId="73"/>
+    <tableColumn id="8" xr3:uid="{1E0CAC48-E2F8-4439-9A70-142378B29E11}" name="ExitWithdrawDate" dataDxfId="72"/>
+    <tableColumn id="9" xr3:uid="{8E363293-A545-4028-86AB-56D402E6B5DF}" name="ExitWithdrawType" dataDxfId="71"/>
+    <tableColumn id="10" xr3:uid="{643BDE56-57B7-44F0-9BF5-CBB7C61DE871}" name="CalendarReference" dataDxfId="70"/>
+    <tableColumn id="11" xr3:uid="{EA285CC7-0C07-4807-BAE0-C470FB431A3C}" name="SpecialEdEvalStatus" dataDxfId="69"/>
+    <tableColumn id="12" xr3:uid="{E4A73A11-17B0-47E2-9CA5-C2E7F1C386F4}" name="StateAidCategory" dataDxfId="68"/>
+    <tableColumn id="13" xr3:uid="{9479A754-4670-458F-9436-083720FA4EBA}" name="HomeboundService" dataDxfId="67"/>
+    <tableColumn id="14" xr3:uid="{C3053064-2B1E-4443-9801-38762BA25785}" name="SpecialPupil" dataDxfId="66"/>
+    <tableColumn id="15" xr3:uid="{6901B54C-5DCF-4EAB-9F58-2FE573BC7343}" name="ResidentLEAReference" dataDxfId="65"/>
+    <tableColumn id="21" xr3:uid="{E301F53A-9DEF-4B90-8299-0DED2B9E40A9}" name="MembershipAttendanceUnit" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{303CB387-33E4-4656-9582-02D45831B388}" name="Attendance" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{0705E415-91EB-4AF5-A47D-97AE74014A06}" name="Membership" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{9846E1C6-D5CD-422C-B9CF-54925AEC931C}" name="PercentEnrolled" dataDxfId="64"/>
+    <tableColumn id="19" xr3:uid="{7730A9C1-1558-4B94-AD1E-5AC7983CABDF}" name="TransportationCategory" dataDxfId="63"/>
+    <tableColumn id="20" xr3:uid="{0E474587-197B-49DB-A30A-C0D1EA91022A}" name="TransportationLEA" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{933DABD0-7C61-4C14-8C2D-7ECEE4DC9E96}" name="SEOAs17" displayName="SEOAs17" ref="A32:P36" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{933DABD0-7C61-4C14-8C2D-7ECEE4DC9E96}" name="SEOAs17" displayName="SEOAs17" ref="A32:P36" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A32:P36" xr:uid="{6534E20D-6A8C-4341-99EF-71275021166D}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{25597A3C-3EA4-44A7-8097-CAAA149E535B}" name="Student" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{495C6C4D-ED0F-4012-849A-F9324268C84F}" name="EdOrgReference SchoolID" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{2044D62F-A399-4D84-97F0-D150BD43357E}" name="StudentUniqueId" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{3B06A6D0-BA8A-44C7-8D57-606D1972BE8E}" name="HispanicLatinoEthnicity" dataDxfId="47"/>
-    <tableColumn id="16" xr3:uid="{282E8BB4-A531-4F14-A37D-A14638E3CCF7}" name="AEO" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{09D96BB6-F2EC-4C98-8AFD-B2CC41648311}" name="Races" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{BE6E30C3-E2E6-498B-BBF6-247C69B37764}" name="Languages" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{3238F1D2-2EBD-4AD6-A8B8-88595FE99E58}" name="LanguageUse" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{43D10D56-20D4-43A4-A346-16EDC4B34B7D}" name="Sex" dataDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{B05CAD9E-363B-4DB4-9216-197F9D00AD4F}" name="StudentCharacteristics" dataDxfId="41"/>
-    <tableColumn id="10" xr3:uid="{F09AAE73-1A66-4872-A5CB-940B5415F101}" name="StudentIdentificationCodes" dataDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{DBBAA6D2-5572-4389-BF8B-9EEEE893F67A}" name="BirthDate" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{77E7AA90-037F-46F3-B330-251D01990E13}" name="FirstName" dataDxfId="38"/>
-    <tableColumn id="13" xr3:uid="{94BEEDD9-E26D-44A8-92B8-FBCC6FDC67DC}" name="MiddleName" dataDxfId="37"/>
-    <tableColumn id="14" xr3:uid="{06D259D8-D6F7-492D-8A6D-085312D3BF49}" name="LastSurname" dataDxfId="36"/>
-    <tableColumn id="15" xr3:uid="{DA761B55-5E97-4A0B-A331-050F6FCAE0A9}" name="OptOutIndicators" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{25597A3C-3EA4-44A7-8097-CAAA149E535B}" name="Student" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{495C6C4D-ED0F-4012-849A-F9324268C84F}" name="EdOrgReference SchoolID" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{2044D62F-A399-4D84-97F0-D150BD43357E}" name="StudentUniqueId" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{3B06A6D0-BA8A-44C7-8D57-606D1972BE8E}" name="HispanicLatinoEthnicity" dataDxfId="56"/>
+    <tableColumn id="16" xr3:uid="{282E8BB4-A531-4F14-A37D-A14638E3CCF7}" name="AEO" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{09D96BB6-F2EC-4C98-8AFD-B2CC41648311}" name="Races" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{BE6E30C3-E2E6-498B-BBF6-247C69B37764}" name="Languages" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{3238F1D2-2EBD-4AD6-A8B8-88595FE99E58}" name="LanguageUse" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{43D10D56-20D4-43A4-A346-16EDC4B34B7D}" name="Sex" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{B05CAD9E-363B-4DB4-9216-197F9D00AD4F}" name="StudentCharacteristics" dataDxfId="50"/>
+    <tableColumn id="10" xr3:uid="{F09AAE73-1A66-4872-A5CB-940B5415F101}" name="StudentIdentificationCodes" dataDxfId="49"/>
+    <tableColumn id="11" xr3:uid="{DBBAA6D2-5572-4389-BF8B-9EEEE893F67A}" name="BirthDate" dataDxfId="48"/>
+    <tableColumn id="12" xr3:uid="{77E7AA90-037F-46F3-B330-251D01990E13}" name="FirstName" dataDxfId="47"/>
+    <tableColumn id="13" xr3:uid="{94BEEDD9-E26D-44A8-92B8-FBCC6FDC67DC}" name="MiddleName" dataDxfId="46"/>
+    <tableColumn id="14" xr3:uid="{06D259D8-D6F7-492D-8A6D-085312D3BF49}" name="LastSurname" dataDxfId="45"/>
+    <tableColumn id="15" xr3:uid="{DA761B55-5E97-4A0B-A331-050F6FCAE0A9}" name="OptOutIndicators" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{56B15117-EF68-47B8-9FDE-F283DEBCB659}" name="SEEPAs18" displayName="SEEPAs18" ref="A40:J44" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{56B15117-EF68-47B8-9FDE-F283DEBCB659}" name="SEEPAs18" displayName="SEEPAs18" ref="A40:J44" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A40:J44" xr:uid="{26630F95-9A06-4446-8DD6-2558045FE47E}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{F9C602C3-335D-445D-8D80-DBCC2538FA70}" name="Student"/>
     <tableColumn id="2" xr3:uid="{E33091ED-F15B-4B45-8406-FD1032C809B3}" name="EdOrgReference SchoolID"/>
     <tableColumn id="3" xr3:uid="{7D335072-A366-47CA-BE62-1060CB51F345}" name="StudentUniqueId"/>
     <tableColumn id="4" xr3:uid="{4FBAD97B-6E30-4838-B1A0-1A5B601E0560}" name="ProgramType"/>
-    <tableColumn id="5" xr3:uid="{1F4A5107-6B4F-4593-BB24-DAFBF459CB86}" name="BeginDate" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{FFA7940C-750A-4FAF-A2EF-04ACEE4BB3B1}" name="EndDate" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{4CC98005-563F-47F2-9D0C-44B3C6F515A7}" name="MembershipAttendanceUnit" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{A6230774-C103-4ECF-AD18-30934165BED7}" name="Attendance" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{6EC83FCF-624B-4B71-BFDD-5C37C18FACC4}" name="Membership" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{31007089-EEE6-4945-ABEE-E51C34B6970B}" name="Percent Enrolled" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{1F4A5107-6B4F-4593-BB24-DAFBF459CB86}" name="BeginDate" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{FFA7940C-750A-4FAF-A2EF-04ACEE4BB3B1}" name="EndDate" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{4CC98005-563F-47F2-9D0C-44B3C6F515A7}" name="MembershipAttendanceUnit" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{A6230774-C103-4ECF-AD18-30934165BED7}" name="Attendance" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{6EC83FCF-624B-4B71-BFDD-5C37C18FACC4}" name="Membership" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{31007089-EEE6-4945-ABEE-E51C34B6970B}" name="Percent Enrolled" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{5692A297-79BF-4F9C-9126-9341754B759A}" name="SEORAs22" displayName="SEORAs22" ref="A24:G28" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{5692A297-79BF-4F9C-9126-9341754B759A}" name="SEORAs22" displayName="SEORAs22" ref="A24:G28" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A24:G28" xr:uid="{77FAAC26-2EEA-45D3-832C-0FF7AB0115F4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:G28">
     <sortCondition ref="A25:A28"/>
     <sortCondition ref="E25:E28"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{97BBDAA1-EEF4-4890-8CC6-F82A47B30DC3}" name="Student" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{E5BB4BAA-D5FE-494C-A12E-4E5CD1FEFE9B}" name="EdOrgReference SchoolID" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{A74DDED4-B75E-4848-97D9-1694DFE7B6C8}" name="StudentUniqueId" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{355E7FFD-F72E-4F56-BD11-829342E8EDCE}" name="ReportingEdOrgReference SchoolID" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{4EA8EC2D-F4E8-4AC9-8F4E-F658A2E86566}" name="BeginDate" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{6F2CC1BA-FBD7-4B28-A91B-22431AA0A9BC}" name="EndDate" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{5D24870A-BBBB-49F7-A22D-9BC354C82EE7}" name="ResponsibiltyDescriptor" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{97BBDAA1-EEF4-4890-8CC6-F82A47B30DC3}" name="Student" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{E5BB4BAA-D5FE-494C-A12E-4E5CD1FEFE9B}" name="EdOrgReference SchoolID" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{A74DDED4-B75E-4848-97D9-1694DFE7B6C8}" name="StudentUniqueId" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{355E7FFD-F72E-4F56-BD11-829342E8EDCE}" name="ReportingEdOrgReference SchoolID" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{4EA8EC2D-F4E8-4AC9-8F4E-F658A2E86566}" name="BeginDate" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{6F2CC1BA-FBD7-4B28-A91B-22431AA0A9BC}" name="EndDate" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{5D24870A-BBBB-49F7-A22D-9BC354C82EE7}" name="ResponsibiltyDescriptor" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{E2C8E32D-19BD-4526-BD62-D5BCA10CC455}" name="EdOrgIds23" displayName="EdOrgIds23" ref="D5:G10" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{E2C8E32D-19BD-4526-BD62-D5BCA10CC455}" name="EdOrgIds23" displayName="EdOrgIds23" ref="D5:G10" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="D5:G10" xr:uid="{E2C8E32D-19BD-4526-BD62-D5BCA10CC455}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FDD8D5C6-800F-4420-AE64-B80892DD5760}" name="Element" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{6E125EEB-7097-4769-8F32-19E6038EE69E}" name="Example ID" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{0922D666-F3DB-47C1-914F-77976F17A1B8}" name="Used In…For this Pattern" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{A977DE9F-420B-4361-B08C-A9FD32195551}" name="Reason" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{FDD8D5C6-800F-4420-AE64-B80892DD5760}" name="Element" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{6E125EEB-7097-4769-8F32-19E6038EE69E}" name="Example ID" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{0922D666-F3DB-47C1-914F-77976F17A1B8}" name="Used In…For this Pattern" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{A977DE9F-420B-4361-B08C-A9FD32195551}" name="Reason" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{8ECA3C70-6EF7-49D0-B684-3D141180DADB}" name="SSEPAs21" displayName="SSEPAs21" ref="A47:J51" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{8ECA3C70-6EF7-49D0-B684-3D141180DADB}" name="SSEPAs21" displayName="SSEPAs21" ref="A47:J51" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A47:J51" xr:uid="{D3CF0901-CC20-4EC6-A4BB-C588254B263D}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{E4DF4947-C3A2-484F-9044-02FFEC2121CC}" name="Student" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{7BAF099E-F389-4EF3-9391-CDA5FEC272D3}" name="EdOrgReference SchoolID" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{01FD7A9A-A19F-48A9-A931-041143D4B550}" name="StudentUniqueId" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{C5888552-F872-4891-82A6-71B6CEFFD6B1}" name="ProgramType" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{2B79307A-550E-4F01-8DD5-FE20AEC09EEF}" name="BeginDate" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{E3D74796-9820-4448-BF45-3877BF979345}" name="EndDate" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{20C673CA-FDFD-4929-A3EA-443A5768000E}" name="DisabilityDescriptor" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{B744BD5D-2FFC-4E93-9A56-B726A607287B}" name="OrderOfDisability" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{CA31B897-F85C-44E1-8EEE-B20CF3FE1A71}" name="SpecialEducationSetting" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{ACB63A65-6385-4A6E-BD2B-697EE91120C2}" name="SpecialEducationServiceHours" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E4DF4947-C3A2-484F-9044-02FFEC2121CC}" name="Student" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{7BAF099E-F389-4EF3-9391-CDA5FEC272D3}" name="EdOrgReference SchoolID" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{01FD7A9A-A19F-48A9-A931-041143D4B550}" name="StudentUniqueId" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{C5888552-F872-4891-82A6-71B6CEFFD6B1}" name="ProgramType" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{2B79307A-550E-4F01-8DD5-FE20AEC09EEF}" name="BeginDate" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{E3D74796-9820-4448-BF45-3877BF979345}" name="EndDate" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{20C673CA-FDFD-4929-A3EA-443A5768000E}" name="DisabilityDescriptor" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{B744BD5D-2FFC-4E93-9A56-B726A607287B}" name="OrderOfDisability" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{CA31B897-F85C-44E1-8EEE-B20CF3FE1A71}" name="SpecialEducationSetting" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{ACB63A65-6385-4A6E-BD2B-697EE91120C2}" name="SpecialEducationServiceHours" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E813628D-9E65-466B-AFAE-06C8ED720622}" name="Students" displayName="Students" ref="A5:B10" totalsRowShown="0" headerRowDxfId="192" dataDxfId="191">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E813628D-9E65-466B-AFAE-06C8ED720622}" name="Students" displayName="Students" ref="A5:B10" totalsRowShown="0" headerRowDxfId="194" dataDxfId="193">
   <autoFilter ref="A5:B10" xr:uid="{E813628D-9E65-466B-AFAE-06C8ED720622}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{509179D6-DE3D-4C78-8484-31CF67D6DDF4}" name="Generic Name" dataDxfId="190"/>
-    <tableColumn id="2" xr3:uid="{6478CE60-2FCB-4233-8C5D-C6E80BE182EC}" name="ID" dataDxfId="189"/>
+    <tableColumn id="1" xr3:uid="{509179D6-DE3D-4C78-8484-31CF67D6DDF4}" name="Generic Name" dataDxfId="192"/>
+    <tableColumn id="2" xr3:uid="{6478CE60-2FCB-4233-8C5D-C6E80BE182EC}" name="ID" dataDxfId="191"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6D6F743E-9CB8-4440-92A1-95FD6FFE6308}" name="Scenarios" displayName="Scenarios" ref="A13:C18" totalsRowShown="0" headerRowDxfId="188" dataDxfId="187">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6D6F743E-9CB8-4440-92A1-95FD6FFE6308}" name="Scenarios" displayName="Scenarios" ref="A13:C18" totalsRowShown="0" headerRowDxfId="190" dataDxfId="189">
   <autoFilter ref="A13:C18" xr:uid="{6D6F743E-9CB8-4440-92A1-95FD6FFE6308}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0C2E717F-6BD2-4A48-8BE9-123940CE8CC5}" name="Scenario Identifier" dataDxfId="186"/>
-    <tableColumn id="3" xr3:uid="{E08C3A90-744B-486E-8E93-AA2AF37C8FB7}" name="Student" dataDxfId="185"/>
-    <tableColumn id="2" xr3:uid="{F14705A2-53EF-4926-AC7C-93386BF8AB53}" name="Description" dataDxfId="184"/>
+    <tableColumn id="1" xr3:uid="{0C2E717F-6BD2-4A48-8BE9-123940CE8CC5}" name="Scenario Identifier" dataDxfId="188"/>
+    <tableColumn id="3" xr3:uid="{E08C3A90-744B-486E-8E93-AA2AF37C8FB7}" name="Student" dataDxfId="187"/>
+    <tableColumn id="2" xr3:uid="{F14705A2-53EF-4926-AC7C-93386BF8AB53}" name="Description" dataDxfId="186"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{85C15CF2-370D-42B8-85DC-039C7BB0A730}" name="SSAs" displayName="SSAs" ref="A21:T30" totalsRowShown="0" headerRowDxfId="183" dataDxfId="182">
-  <autoFilter ref="A21:T30" xr:uid="{85C15CF2-370D-42B8-85DC-039C7BB0A730}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:T30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{85C15CF2-370D-42B8-85DC-039C7BB0A730}" name="SSAs" displayName="SSAs" ref="A21:U30" totalsRowShown="0" headerRowDxfId="185" dataDxfId="184">
+  <autoFilter ref="A21:U30" xr:uid="{85C15CF2-370D-42B8-85DC-039C7BB0A730}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:U30">
     <sortCondition ref="A22:A30"/>
     <sortCondition ref="E22:E30"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{20DF5C0D-B071-41B9-9108-59CC1676781B}" name="Student" dataDxfId="181"/>
-    <tableColumn id="2" xr3:uid="{E4DC74D4-A5B4-426C-92CB-09562E49B40A}" name="SchoolYear" dataDxfId="180"/>
-    <tableColumn id="3" xr3:uid="{560EC4E5-E4DF-4EF2-8F1B-513A68FB240F}" name="SchoolReference SchoolID" dataDxfId="179"/>
-    <tableColumn id="4" xr3:uid="{E69278B1-3248-4F61-9E2C-E196F9CC4716}" name="StudentUniqueId" dataDxfId="178"/>
-    <tableColumn id="5" xr3:uid="{0B177AFA-A9E4-442F-98B9-5318B9FE526B}" name="EntryDate" dataDxfId="177"/>
-    <tableColumn id="6" xr3:uid="{4E48BB48-3EC0-4F71-9B97-DEA44D8944C0}" name="EntryType" dataDxfId="176"/>
-    <tableColumn id="7" xr3:uid="{F182D772-DCF0-4B88-A29F-660C049B056B}" name="EntryGradeLevel" dataDxfId="175"/>
-    <tableColumn id="8" xr3:uid="{8C905914-751D-415D-A4B5-1CCAE96B1C8D}" name="ExitWithdrawDate" dataDxfId="174"/>
-    <tableColumn id="9" xr3:uid="{30F96063-E712-4EBA-B137-4167E5A3651B}" name="ExitWithdrawType" dataDxfId="173"/>
-    <tableColumn id="10" xr3:uid="{B8E2A9FC-7483-42CF-A097-D17A0779FE76}" name="CalendarReference" dataDxfId="172"/>
-    <tableColumn id="11" xr3:uid="{553AA797-93D6-4CAE-A81C-8DEBED9C5953}" name="SpecialEdEvalStatus" dataDxfId="171"/>
-    <tableColumn id="12" xr3:uid="{8E016F3E-0D81-406E-A517-13FEC26F87FB}" name="StateAidCategory" dataDxfId="170"/>
-    <tableColumn id="13" xr3:uid="{F73F852B-30BA-444D-8002-FB95BD31D484}" name="HomeboundService" dataDxfId="169"/>
-    <tableColumn id="14" xr3:uid="{8CF7231E-E453-476C-80A5-696516A4E92E}" name="SpecialPupil" dataDxfId="168"/>
-    <tableColumn id="15" xr3:uid="{54611861-C7B1-4E49-9D59-FA95E3AA1DDF}" name="ResidentLEAReference" dataDxfId="167"/>
-    <tableColumn id="16" xr3:uid="{B00E0262-A73E-40C6-A2D1-5C01FEA1382D}" name="AttendanceDays" dataDxfId="166"/>
-    <tableColumn id="17" xr3:uid="{4F7FD020-423E-4DAC-BACD-27A9147BB8D0}" name="MembershipDays" dataDxfId="165"/>
-    <tableColumn id="18" xr3:uid="{9344241F-6C08-4119-A8BB-6C4A3BBD67D9}" name="PercentEnrolled" dataDxfId="164"/>
-    <tableColumn id="19" xr3:uid="{C050E003-D9FE-4A89-AD1F-B5B18A6BFAC3}" name="TransportationCategory" dataDxfId="163"/>
-    <tableColumn id="20" xr3:uid="{0692C374-1DB3-497F-8B1D-3728A0D56DE2}" name="TransportationLEA" dataDxfId="162"/>
+  <tableColumns count="21">
+    <tableColumn id="1" xr3:uid="{20DF5C0D-B071-41B9-9108-59CC1676781B}" name="Student" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{E4DC74D4-A5B4-426C-92CB-09562E49B40A}" name="SchoolYear" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{560EC4E5-E4DF-4EF2-8F1B-513A68FB240F}" name="SchoolReference SchoolID" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{E69278B1-3248-4F61-9E2C-E196F9CC4716}" name="StudentUniqueId" dataDxfId="180"/>
+    <tableColumn id="5" xr3:uid="{0B177AFA-A9E4-442F-98B9-5318B9FE526B}" name="EntryDate" dataDxfId="179"/>
+    <tableColumn id="6" xr3:uid="{4E48BB48-3EC0-4F71-9B97-DEA44D8944C0}" name="EntryType" dataDxfId="178"/>
+    <tableColumn id="7" xr3:uid="{F182D772-DCF0-4B88-A29F-660C049B056B}" name="EntryGradeLevel" dataDxfId="177"/>
+    <tableColumn id="8" xr3:uid="{8C905914-751D-415D-A4B5-1CCAE96B1C8D}" name="ExitWithdrawDate" dataDxfId="176"/>
+    <tableColumn id="9" xr3:uid="{30F96063-E712-4EBA-B137-4167E5A3651B}" name="ExitWithdrawType" dataDxfId="175"/>
+    <tableColumn id="10" xr3:uid="{B8E2A9FC-7483-42CF-A097-D17A0779FE76}" name="CalendarReference" dataDxfId="174"/>
+    <tableColumn id="11" xr3:uid="{553AA797-93D6-4CAE-A81C-8DEBED9C5953}" name="SpecialEdEvalStatus" dataDxfId="173"/>
+    <tableColumn id="12" xr3:uid="{8E016F3E-0D81-406E-A517-13FEC26F87FB}" name="StateAidCategory" dataDxfId="172"/>
+    <tableColumn id="13" xr3:uid="{F73F852B-30BA-444D-8002-FB95BD31D484}" name="HomeboundService" dataDxfId="171"/>
+    <tableColumn id="14" xr3:uid="{8CF7231E-E453-476C-80A5-696516A4E92E}" name="SpecialPupil" dataDxfId="170"/>
+    <tableColumn id="15" xr3:uid="{54611861-C7B1-4E49-9D59-FA95E3AA1DDF}" name="ResidentLEAReference" dataDxfId="169"/>
+    <tableColumn id="21" xr3:uid="{438C1F18-E0A0-4604-A90C-3B2A4F7690BF}" name="MembershipAttendanceUnit" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{B00E0262-A73E-40C6-A2D1-5C01FEA1382D}" name="Attendance" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{4F7FD020-423E-4DAC-BACD-27A9147BB8D0}" name="Membership" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{9344241F-6C08-4119-A8BB-6C4A3BBD67D9}" name="PercentEnrolled" dataDxfId="8"/>
+    <tableColumn id="19" xr3:uid="{C050E003-D9FE-4A89-AD1F-B5B18A6BFAC3}" name="TransportationCategory" dataDxfId="168"/>
+    <tableColumn id="20" xr3:uid="{0692C374-1DB3-497F-8B1D-3728A0D56DE2}" name="TransportationLEA" dataDxfId="167"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F2BCDEC8-8E36-4C36-BE66-F0CF6D0EC644}" name="EdOrgIds" displayName="EdOrgIds" ref="D5:G10" totalsRowShown="0" headerRowDxfId="161" dataDxfId="160">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F2BCDEC8-8E36-4C36-BE66-F0CF6D0EC644}" name="EdOrgIds" displayName="EdOrgIds" ref="D5:G10" totalsRowShown="0" headerRowDxfId="166" dataDxfId="165">
   <autoFilter ref="D5:G10" xr:uid="{F2BCDEC8-8E36-4C36-BE66-F0CF6D0EC644}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8E85224E-E7A7-4FE6-8296-B643291CD515}" name="Element" dataDxfId="159"/>
-    <tableColumn id="2" xr3:uid="{82CD4B99-8DFA-476D-9708-9EE44D5FEEED}" name="Example ID" dataDxfId="158"/>
-    <tableColumn id="4" xr3:uid="{093AD196-E421-4873-8CF7-8828F582DC33}" name="Used In…For this Pattern" dataDxfId="157"/>
-    <tableColumn id="3" xr3:uid="{C1A37B0E-9E2F-4A1D-9EB8-4B6289B3EF5C}" name="Reason" dataDxfId="156"/>
+    <tableColumn id="1" xr3:uid="{8E85224E-E7A7-4FE6-8296-B643291CD515}" name="Element" dataDxfId="164"/>
+    <tableColumn id="2" xr3:uid="{82CD4B99-8DFA-476D-9708-9EE44D5FEEED}" name="Example ID" dataDxfId="163"/>
+    <tableColumn id="4" xr3:uid="{093AD196-E421-4873-8CF7-8828F582DC33}" name="Used In…For this Pattern" dataDxfId="162"/>
+    <tableColumn id="3" xr3:uid="{C1A37B0E-9E2F-4A1D-9EB8-4B6289B3EF5C}" name="Reason" dataDxfId="161"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6534E20D-6A8C-4341-99EF-71275021166D}" name="SEOAs" displayName="SEOAs" ref="A46:P51" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6534E20D-6A8C-4341-99EF-71275021166D}" name="SEOAs" displayName="SEOAs" ref="A46:P51" totalsRowShown="0" headerRowDxfId="160" dataDxfId="159">
   <autoFilter ref="A46:P51" xr:uid="{6534E20D-6A8C-4341-99EF-71275021166D}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{A4A3D2FA-EDEE-45D8-9A6E-286AEB0C5BAF}" name="Student" dataDxfId="153"/>
-    <tableColumn id="2" xr3:uid="{A4F12726-9355-482E-ACB5-BD97FDC71288}" name="EdOrgReference SchoolID" dataDxfId="152"/>
-    <tableColumn id="3" xr3:uid="{A43CAF59-3D92-41B2-8921-8D26AF385820}" name="StudentUniqueId" dataDxfId="151"/>
-    <tableColumn id="4" xr3:uid="{A1FC7C2A-8C5E-45CD-B0EC-3011A475BBF6}" name="HispanicLatinoEthnicity" dataDxfId="150"/>
-    <tableColumn id="16" xr3:uid="{7F867879-6DD8-4834-9F9C-F40372F0D69F}" name="AEO" dataDxfId="149"/>
-    <tableColumn id="5" xr3:uid="{88E4A252-66D7-440E-B436-F96D57455583}" name="Races" dataDxfId="148"/>
-    <tableColumn id="6" xr3:uid="{53538A8D-8B3E-45DC-A3BE-6E64C28691A4}" name="Languages" dataDxfId="147"/>
-    <tableColumn id="7" xr3:uid="{D23E5EE2-E77E-457E-8165-58CE95E357EA}" name="LanguageUse" dataDxfId="146"/>
-    <tableColumn id="8" xr3:uid="{8679C1C7-0B37-4284-BF26-B514074CA756}" name="Sex" dataDxfId="145"/>
-    <tableColumn id="9" xr3:uid="{2A8D3774-405C-4EC5-A4E9-FE6BCC9ADE70}" name="StudentCharacteristics" dataDxfId="144"/>
-    <tableColumn id="10" xr3:uid="{542FCA80-189D-4AEE-855C-31A39E5EB85B}" name="StudentIdentificationCodes" dataDxfId="143"/>
-    <tableColumn id="11" xr3:uid="{3CB29F9B-A7A6-4565-B260-2906AF84129F}" name="BirthDate" dataDxfId="142"/>
-    <tableColumn id="12" xr3:uid="{080B3624-FBF4-45A9-A4CC-0698348072EE}" name="FirstName" dataDxfId="141"/>
-    <tableColumn id="13" xr3:uid="{F42D074E-6F35-489F-8757-9F408445D91C}" name="MiddleName" dataDxfId="140"/>
-    <tableColumn id="14" xr3:uid="{B839DA8B-9F76-46DA-9A57-B55DB230E6CA}" name="LastSurname" dataDxfId="139"/>
-    <tableColumn id="15" xr3:uid="{D6DFBB36-E469-4FB9-A50A-3ED2BDAD3CC4}" name="OptOutIndicators" dataDxfId="138"/>
+    <tableColumn id="1" xr3:uid="{A4A3D2FA-EDEE-45D8-9A6E-286AEB0C5BAF}" name="Student" dataDxfId="158"/>
+    <tableColumn id="2" xr3:uid="{A4F12726-9355-482E-ACB5-BD97FDC71288}" name="EdOrgReference SchoolID" dataDxfId="157"/>
+    <tableColumn id="3" xr3:uid="{A43CAF59-3D92-41B2-8921-8D26AF385820}" name="StudentUniqueId" dataDxfId="156"/>
+    <tableColumn id="4" xr3:uid="{A1FC7C2A-8C5E-45CD-B0EC-3011A475BBF6}" name="HispanicLatinoEthnicity" dataDxfId="155"/>
+    <tableColumn id="16" xr3:uid="{7F867879-6DD8-4834-9F9C-F40372F0D69F}" name="AEO" dataDxfId="154"/>
+    <tableColumn id="5" xr3:uid="{88E4A252-66D7-440E-B436-F96D57455583}" name="Races" dataDxfId="153"/>
+    <tableColumn id="6" xr3:uid="{53538A8D-8B3E-45DC-A3BE-6E64C28691A4}" name="Languages" dataDxfId="152"/>
+    <tableColumn id="7" xr3:uid="{D23E5EE2-E77E-457E-8165-58CE95E357EA}" name="LanguageUse" dataDxfId="151"/>
+    <tableColumn id="8" xr3:uid="{8679C1C7-0B37-4284-BF26-B514074CA756}" name="Sex" dataDxfId="150"/>
+    <tableColumn id="9" xr3:uid="{2A8D3774-405C-4EC5-A4E9-FE6BCC9ADE70}" name="StudentCharacteristics" dataDxfId="149"/>
+    <tableColumn id="10" xr3:uid="{542FCA80-189D-4AEE-855C-31A39E5EB85B}" name="StudentIdentificationCodes" dataDxfId="148"/>
+    <tableColumn id="11" xr3:uid="{3CB29F9B-A7A6-4565-B260-2906AF84129F}" name="BirthDate" dataDxfId="147"/>
+    <tableColumn id="12" xr3:uid="{080B3624-FBF4-45A9-A4CC-0698348072EE}" name="FirstName" dataDxfId="146"/>
+    <tableColumn id="13" xr3:uid="{F42D074E-6F35-489F-8757-9F408445D91C}" name="MiddleName" dataDxfId="145"/>
+    <tableColumn id="14" xr3:uid="{B839DA8B-9F76-46DA-9A57-B55DB230E6CA}" name="LastSurname" dataDxfId="144"/>
+    <tableColumn id="15" xr3:uid="{D6DFBB36-E469-4FB9-A50A-3ED2BDAD3CC4}" name="OptOutIndicators" dataDxfId="143"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{26630F95-9A06-4446-8DD6-2558045FE47E}" name="SEEPAs" displayName="SEEPAs" ref="A55:J56" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{26630F95-9A06-4446-8DD6-2558045FE47E}" name="SEEPAs" displayName="SEEPAs" ref="A55:J56" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141">
   <autoFilter ref="A55:J56" xr:uid="{26630F95-9A06-4446-8DD6-2558045FE47E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F4C6ABD2-814B-4123-8E5A-62079CA8844E}" name="Student" dataDxfId="135"/>
-    <tableColumn id="2" xr3:uid="{B47E9466-2F59-40DC-BC6B-CCAFF687EA9F}" name="EdOrgReference SchoolID" dataDxfId="134"/>
-    <tableColumn id="3" xr3:uid="{13703732-AC7D-4B9C-AE0A-35BCC984E0F3}" name="StudentUniqueId" dataDxfId="133"/>
-    <tableColumn id="4" xr3:uid="{53FFB636-DB86-49B1-AA7D-9F15D7AEBACE}" name="ProgramType" dataDxfId="132"/>
-    <tableColumn id="5" xr3:uid="{8F49C286-C71C-4CAB-B47B-68D3411F7ECE}" name="BeginDate" dataDxfId="131"/>
-    <tableColumn id="6" xr3:uid="{2F2AFF46-9F5C-4FE0-B496-DF6C18DE9E8A}" name="EndDate" dataDxfId="130"/>
-    <tableColumn id="7" xr3:uid="{1C8C41F3-0DAB-49F7-B6A8-64F735833315}" name="MembershipAttendanceUnit" dataDxfId="129"/>
-    <tableColumn id="8" xr3:uid="{32BDBBC3-62E9-4D26-99AF-88573C5F627F}" name="Attendance" dataDxfId="128"/>
-    <tableColumn id="9" xr3:uid="{C723C480-F019-464D-9822-41DCD668AC80}" name="Membership" dataDxfId="127"/>
-    <tableColumn id="10" xr3:uid="{1067938B-0918-498E-9584-5C9C2E812DE2}" name="Percent Enrolled" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{F4C6ABD2-814B-4123-8E5A-62079CA8844E}" name="Student" dataDxfId="140"/>
+    <tableColumn id="2" xr3:uid="{B47E9466-2F59-40DC-BC6B-CCAFF687EA9F}" name="EdOrgReference SchoolID" dataDxfId="139"/>
+    <tableColumn id="3" xr3:uid="{13703732-AC7D-4B9C-AE0A-35BCC984E0F3}" name="StudentUniqueId" dataDxfId="138"/>
+    <tableColumn id="4" xr3:uid="{53FFB636-DB86-49B1-AA7D-9F15D7AEBACE}" name="ProgramType" dataDxfId="137"/>
+    <tableColumn id="5" xr3:uid="{8F49C286-C71C-4CAB-B47B-68D3411F7ECE}" name="BeginDate" dataDxfId="136"/>
+    <tableColumn id="6" xr3:uid="{2F2AFF46-9F5C-4FE0-B496-DF6C18DE9E8A}" name="EndDate" dataDxfId="135"/>
+    <tableColumn id="7" xr3:uid="{1C8C41F3-0DAB-49F7-B6A8-64F735833315}" name="MembershipAttendanceUnit" dataDxfId="134"/>
+    <tableColumn id="8" xr3:uid="{32BDBBC3-62E9-4D26-99AF-88573C5F627F}" name="Attendance" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{C723C480-F019-464D-9822-41DCD668AC80}" name="Membership" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{1067938B-0918-498E-9584-5C9C2E812DE2}" name="Percent Enrolled" dataDxfId="133"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CE1A2133-3BCA-425D-8B3A-B8B9EC1563A6}" name="SHPAs" displayName="SHPAs" ref="A59:H60" totalsRowShown="0" headerRowDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CE1A2133-3BCA-425D-8B3A-B8B9EC1563A6}" name="SHPAs" displayName="SHPAs" ref="A59:H60" totalsRowShown="0" headerRowDxfId="132">
   <autoFilter ref="A59:H60" xr:uid="{CE1A2133-3BCA-425D-8B3A-B8B9EC1563A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{04F78B13-55C3-43E3-95AF-59AF667F7DFB}" name="Student" dataDxfId="124"/>
-    <tableColumn id="2" xr3:uid="{7AE0FA1D-F422-466D-BE2F-56A5145E58EF}" name="EdOrgReference SchoolID" dataDxfId="123"/>
-    <tableColumn id="3" xr3:uid="{D8E0F478-4BB1-43DC-92E9-40EDF28DCFF2}" name="StudentUniqueId" dataDxfId="122"/>
-    <tableColumn id="4" xr3:uid="{ABC62F79-6030-4B33-A9EF-ABF1DC62BE62}" name="ProgramType" dataDxfId="121"/>
-    <tableColumn id="5" xr3:uid="{0634D05E-EB78-4F6C-A8B2-10BC6D46DB5C}" name="BeginDate" dataDxfId="120"/>
-    <tableColumn id="6" xr3:uid="{44F548B9-8217-43E0-B167-4C6D4A84F092}" name="EndDate" dataDxfId="119"/>
-    <tableColumn id="7" xr3:uid="{30CFA4E9-CEE8-4738-B52D-510A0602B8D4}" name="PrimaryNighttimeResidence" dataDxfId="118"/>
-    <tableColumn id="8" xr3:uid="{908C03ED-48BA-4124-B77C-EB692F9777B2}" name="Unaccompanied" dataDxfId="117"/>
+    <tableColumn id="1" xr3:uid="{04F78B13-55C3-43E3-95AF-59AF667F7DFB}" name="Student" dataDxfId="131"/>
+    <tableColumn id="2" xr3:uid="{7AE0FA1D-F422-466D-BE2F-56A5145E58EF}" name="EdOrgReference SchoolID" dataDxfId="130"/>
+    <tableColumn id="3" xr3:uid="{D8E0F478-4BB1-43DC-92E9-40EDF28DCFF2}" name="StudentUniqueId" dataDxfId="129"/>
+    <tableColumn id="4" xr3:uid="{ABC62F79-6030-4B33-A9EF-ABF1DC62BE62}" name="ProgramType" dataDxfId="128"/>
+    <tableColumn id="5" xr3:uid="{0634D05E-EB78-4F6C-A8B2-10BC6D46DB5C}" name="BeginDate" dataDxfId="127"/>
+    <tableColumn id="6" xr3:uid="{44F548B9-8217-43E0-B167-4C6D4A84F092}" name="EndDate" dataDxfId="126"/>
+    <tableColumn id="7" xr3:uid="{30CFA4E9-CEE8-4738-B52D-510A0602B8D4}" name="PrimaryNighttimeResidence" dataDxfId="125"/>
+    <tableColumn id="8" xr3:uid="{908C03ED-48BA-4124-B77C-EB692F9777B2}" name="Unaccompanied" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D73DF4A3-0B69-423F-AE1A-12C79E70A91B}" name="SSFSPAs" displayName="SSFSPAs" ref="A63:I71" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D73DF4A3-0B69-423F-AE1A-12C79E70A91B}" name="SSFSPAs" displayName="SSFSPAs" ref="A63:I71" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
   <autoFilter ref="A63:I71" xr:uid="{D73DF4A3-0B69-423F-AE1A-12C79E70A91B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6726B54E-590F-4630-B499-DF209BD6B268}" name="Student" dataDxfId="114"/>
-    <tableColumn id="2" xr3:uid="{A04B0A75-89FE-461C-9F22-40FC8BBE7988}" name="EdOrgReference SchoolID" dataDxfId="113"/>
-    <tableColumn id="3" xr3:uid="{7C3FAEFA-56A7-41F9-8E6F-CA76242BEEE2}" name="StudentUniqueId" dataDxfId="112"/>
-    <tableColumn id="4" xr3:uid="{2FF748BD-2F0E-4FF7-8B34-0F37E874D63E}" name="ProgramType" dataDxfId="111"/>
-    <tableColumn id="5" xr3:uid="{5E2E2E38-8BB5-4561-BD41-B7C7C5644445}" name="BeginDate" dataDxfId="110"/>
-    <tableColumn id="6" xr3:uid="{C597EBBD-6F81-400F-AAA1-7E35A1A81904}" name="EndDate" dataDxfId="109"/>
-    <tableColumn id="7" xr3:uid="{5AF3867E-7461-42FB-B199-114ABC8D724C}" name="Direct Certification" dataDxfId="108"/>
-    <tableColumn id="8" xr3:uid="{60A3ECAD-2AF3-45D7-ACE7-7F63BCAE08DC}" name="School Food Service Program Service" dataDxfId="107"/>
-    <tableColumn id="9" xr3:uid="{725AB688-A37C-47F1-BCBD-ED89B3141417}" name="Notes" dataDxfId="106"/>
+    <tableColumn id="1" xr3:uid="{6726B54E-590F-4630-B499-DF209BD6B268}" name="Student" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{A04B0A75-89FE-461C-9F22-40FC8BBE7988}" name="EdOrgReference SchoolID" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{7C3FAEFA-56A7-41F9-8E6F-CA76242BEEE2}" name="StudentUniqueId" dataDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{2FF748BD-2F0E-4FF7-8B34-0F37E874D63E}" name="ProgramType" dataDxfId="118"/>
+    <tableColumn id="5" xr3:uid="{5E2E2E38-8BB5-4561-BD41-B7C7C5644445}" name="BeginDate" dataDxfId="117"/>
+    <tableColumn id="6" xr3:uid="{C597EBBD-6F81-400F-AAA1-7E35A1A81904}" name="EndDate" dataDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{5AF3867E-7461-42FB-B199-114ABC8D724C}" name="Direct Certification" dataDxfId="115"/>
+    <tableColumn id="8" xr3:uid="{60A3ECAD-2AF3-45D7-ACE7-7F63BCAE08DC}" name="School Food Service Program Service" dataDxfId="114"/>
+    <tableColumn id="9" xr3:uid="{725AB688-A37C-47F1-BCBD-ED89B3141417}" name="Notes" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5262,28 +5262,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="P21" dT="2024-05-09T18:04:25.87" personId="{64E8492C-03DE-4998-8505-BC99EAD32963}" id="{53C709BC-7C1F-4D55-A8EB-3519CF26184E}">
-    <text>Are we really only dealing in days for membership and attendance?</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="P17" dT="2024-05-09T18:04:25.87" personId="{64E8492C-03DE-4998-8505-BC99EAD32963}" id="{BFCB5ABF-48BF-4194-8828-6EA40B2FEB51}">
-    <text>Are we really only dealing in days for membership and attendance?</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA5FF19-54A6-4517-A0A6-3EE6F2194B71}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5298,12 +5282,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -5318,7 +5302,7 @@
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -5327,20 +5311,20 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="17"/>
@@ -5349,7 +5333,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -5357,7 +5341,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="2"/>
@@ -5365,7 +5349,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="2"/>
@@ -5373,7 +5357,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="2"/>
@@ -5381,7 +5365,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="2"/>
@@ -5405,7 +5389,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -5414,7 +5398,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -5430,7 +5414,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>0</v>
@@ -5453,19 +5437,19 @@
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -5476,16 +5460,16 @@
         <v>44</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -5493,19 +5477,19 @@
         <v>3</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="F20" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -5513,19 +5497,19 @@
         <v>4</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -5541,11 +5525,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136FD443-4433-4AA8-9391-F8565D648BB7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136FD443-4433-4AA8-9391-F8565D648BB7}">
   <dimension ref="A1:W96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5565,7 +5549,7 @@
     <col min="13" max="13" width="21" style="2" customWidth="1"/>
     <col min="14" max="14" width="16.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="18" style="2" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="2" customWidth="1"/>
     <col min="18" max="18" width="17.85546875" style="2" customWidth="1"/>
     <col min="19" max="19" width="24.42578125" style="2" customWidth="1"/>
@@ -5575,10 +5559,10 @@
   <sheetData>
     <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5587,7 +5571,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E3" s="10"/>
     </row>
@@ -5616,7 +5600,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>40</v>
@@ -5632,16 +5616,16 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E6" s="2">
         <v>10271000</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="W6" s="2"/>
     </row>
@@ -5660,10 +5644,10 @@
         <v>60917000</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="W7" s="2"/>
     </row>
@@ -5676,16 +5660,16 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E8" s="2">
         <v>10271009</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="W8" s="2"/>
     </row>
@@ -5704,10 +5688,10 @@
         <v>60917030</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="W9" s="2"/>
     </row>
@@ -5720,14 +5704,14 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="W10" s="2"/>
     </row>
@@ -5787,7 +5771,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -5798,7 +5782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -5809,13 +5793,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:20" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:21" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -5844,7 +5828,7 @@
         <v>50</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>51</v>
@@ -5862,22 +5846,25 @@
         <v>55</v>
       </c>
       <c r="P21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="T21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="R21" s="2" t="s">
+      <c r="U21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="S21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -5906,7 +5893,7 @@
         <v>99</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K22" s="2">
         <v>4</v>
@@ -5915,31 +5902,34 @@
         <v>46</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O22" s="2">
         <v>10271000</v>
       </c>
-      <c r="P22" s="2">
+      <c r="P22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q22" s="19">
         <v>0</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="R22" s="20">
         <v>0</v>
       </c>
-      <c r="R22" s="2">
+      <c r="S22" s="2">
         <v>100</v>
       </c>
-      <c r="S22" s="2">
+      <c r="T22" s="2">
         <v>0</v>
       </c>
-      <c r="T22" s="2">
+      <c r="U22" s="2">
         <v>10271000</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -5968,7 +5958,7 @@
         <v>8</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K23" s="2">
         <v>4</v>
@@ -5977,31 +5967,34 @@
         <v>19</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O23" s="2">
         <v>10271000</v>
       </c>
-      <c r="P23" s="2">
-        <v>1510</v>
-      </c>
-      <c r="Q23" s="2">
+      <c r="P23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q23" s="19">
+        <v>151</v>
+      </c>
+      <c r="R23" s="20">
         <v>168</v>
       </c>
-      <c r="R23" s="2">
+      <c r="S23" s="2">
         <v>100</v>
       </c>
-      <c r="S23" s="2">
+      <c r="T23" s="2">
         <v>3</v>
       </c>
-      <c r="T23" s="2">
+      <c r="U23" s="2">
         <v>10271000</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -6030,7 +6023,7 @@
         <v>99</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K24" s="2">
         <v>1</v>
@@ -6039,31 +6032,34 @@
         <v>77</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O24" s="2">
         <v>10194000</v>
       </c>
-      <c r="P24" s="2">
-        <v>130</v>
-      </c>
-      <c r="Q24" s="2">
+      <c r="P24" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q24" s="19">
         <v>13</v>
       </c>
-      <c r="R24" s="2">
+      <c r="R24" s="20">
+        <v>13</v>
+      </c>
+      <c r="S24" s="2">
         <v>999</v>
       </c>
-      <c r="S24" s="2">
+      <c r="T24" s="2">
         <v>0</v>
       </c>
-      <c r="T24" s="2">
+      <c r="U24" s="2">
         <v>10194000</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -6092,7 +6088,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K25" s="2">
         <v>4</v>
@@ -6101,31 +6097,34 @@
         <v>27</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O25" s="2">
         <v>10194000</v>
       </c>
-      <c r="P25" s="2">
-        <v>950</v>
-      </c>
-      <c r="Q25" s="2">
+      <c r="P25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q25" s="19">
         <v>95</v>
       </c>
-      <c r="R25" s="2">
+      <c r="R25" s="20">
+        <v>95</v>
+      </c>
+      <c r="S25" s="2">
         <v>999</v>
       </c>
-      <c r="S25" s="2">
+      <c r="T25" s="2">
         <v>0</v>
       </c>
-      <c r="T25" s="2">
+      <c r="U25" s="2">
         <v>10194000</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -6154,7 +6153,7 @@
         <v>99</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K26" s="2">
         <v>4</v>
@@ -6163,31 +6162,34 @@
         <v>27</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O26" s="2">
         <v>10199000</v>
       </c>
-      <c r="P26" s="2">
-        <v>1055</v>
-      </c>
-      <c r="Q26" s="2">
+      <c r="P26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q26" s="19">
+        <v>105.5</v>
+      </c>
+      <c r="R26" s="20">
         <v>106</v>
       </c>
-      <c r="R26" s="2">
+      <c r="S26" s="2">
         <v>999</v>
       </c>
-      <c r="S26" s="2">
+      <c r="T26" s="2">
         <v>0</v>
       </c>
-      <c r="T26" s="2">
+      <c r="U26" s="2">
         <v>10199000</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -6216,7 +6218,7 @@
         <v>40</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K27" s="2">
         <v>4</v>
@@ -6225,31 +6227,34 @@
         <v>27</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O27" s="2">
         <v>10199000</v>
       </c>
-      <c r="P27" s="2">
-        <v>5653</v>
-      </c>
-      <c r="Q27" s="2">
+      <c r="P27" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q27" s="19">
+        <v>565.29999999999995</v>
+      </c>
+      <c r="R27" s="20">
         <v>627</v>
       </c>
-      <c r="R27" s="2">
+      <c r="S27" s="2">
         <v>999</v>
       </c>
-      <c r="S27" s="2">
+      <c r="T27" s="2">
         <v>6</v>
       </c>
-      <c r="T27" s="2">
+      <c r="U27" s="2">
         <v>10199000</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -6269,7 +6274,7 @@
         <v>4</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H28" s="8">
         <v>45436</v>
@@ -6278,7 +6283,7 @@
         <v>40</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K28" s="2">
         <v>4</v>
@@ -6287,31 +6292,34 @@
         <v>19</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O28" s="2">
         <v>10271000</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>63</v>
+        <v>151</v>
+      </c>
+      <c r="Q28" s="19">
+        <v>46</v>
+      </c>
+      <c r="R28" s="20">
+        <v>59</v>
       </c>
       <c r="S28" s="2">
+        <v>999</v>
+      </c>
+      <c r="T28" s="2">
         <v>3</v>
       </c>
-      <c r="T28" s="2">
+      <c r="U28" s="2">
         <v>10271000</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -6340,7 +6348,7 @@
         <v>99</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K29" s="2">
         <v>1</v>
@@ -6349,31 +6357,34 @@
         <v>3</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O29" s="2">
         <v>10199000</v>
       </c>
-      <c r="P29" s="2">
-        <v>2131</v>
-      </c>
-      <c r="Q29" s="2">
+      <c r="P29" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q29" s="19">
+        <v>213.1</v>
+      </c>
+      <c r="R29" s="20">
         <v>258</v>
       </c>
-      <c r="R29" s="2">
+      <c r="S29" s="2">
         <v>999</v>
       </c>
-      <c r="S29" s="2">
+      <c r="T29" s="2">
         <v>0</v>
       </c>
-      <c r="T29" s="2">
+      <c r="U29" s="2">
         <v>10199000</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -6402,7 +6413,7 @@
         <v>40</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K30" s="2">
         <v>1</v>
@@ -6411,34 +6422,37 @@
         <v>3</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O30" s="2">
         <v>10199000</v>
       </c>
-      <c r="P30" s="2">
-        <v>5928</v>
-      </c>
-      <c r="Q30" s="2">
+      <c r="P30" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q30" s="19">
+        <v>592.79999999999995</v>
+      </c>
+      <c r="R30" s="20">
         <v>780</v>
       </c>
-      <c r="R30" s="2">
+      <c r="S30" s="2">
         <v>999</v>
       </c>
-      <c r="S30" s="2">
+      <c r="T30" s="2">
         <v>0</v>
       </c>
-      <c r="T30" s="2">
+      <c r="U30" s="2">
         <v>10199000</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:20" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:21" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6446,22 +6460,22 @@
         <v>20</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6484,7 +6498,7 @@
         <v>45141</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6507,7 +6521,7 @@
         <v>45442</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6530,7 +6544,7 @@
         <v>45142</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6553,7 +6567,7 @@
         <v>45216</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6576,7 +6590,7 @@
         <v>45216</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6599,7 +6613,7 @@
         <v>45449</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6622,7 +6636,7 @@
         <v>45436</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6645,7 +6659,7 @@
         <v>45238</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6668,7 +6682,7 @@
         <v>45449</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6677,12 +6691,12 @@
     </row>
     <row r="44" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6690,49 +6704,49 @@
         <v>20</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K46" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H46" s="2" t="s">
+      <c r="L46" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J46" s="2" t="s">
+      <c r="M46" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="N46" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="O46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M46" s="2" t="s">
+      <c r="P46" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6746,40 +6760,40 @@
         <v>8</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G47" s="2">
         <v>11</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L47" s="8">
         <v>37560</v>
       </c>
       <c r="M47" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N47" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O47" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6793,40 +6807,40 @@
         <v>16</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G48" s="2">
         <v>11</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L48" s="8">
         <v>39007</v>
       </c>
       <c r="M48" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N48" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O48" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6840,40 +6854,40 @@
         <v>17</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G49" s="2">
         <v>11</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L49" s="8">
         <v>39062</v>
       </c>
       <c r="M49" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N49" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O49" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6887,40 +6901,40 @@
         <v>18</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G50" s="2">
         <v>11</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L50" s="8">
         <v>43455</v>
       </c>
       <c r="M50" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N50" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O50" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6934,50 +6948,50 @@
         <v>19</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G51" s="2">
         <v>11</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L51" s="8">
         <v>39024</v>
       </c>
       <c r="M51" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N51" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O51" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6985,28 +6999,28 @@
         <v>20</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E55" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>37</v>
@@ -7023,7 +7037,7 @@
         <v>18</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E56" s="8">
         <v>45261</v>
@@ -7032,13 +7046,13 @@
         <v>45436</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H56" s="2">
-        <v>2525</v>
-      </c>
-      <c r="I56" s="2">
-        <v>258</v>
+        <v>151</v>
+      </c>
+      <c r="H56" s="19">
+        <v>46</v>
+      </c>
+      <c r="I56" s="20">
+        <v>59</v>
       </c>
       <c r="J56" s="2">
         <v>999</v>
@@ -7050,10 +7064,10 @@
     </row>
     <row r="58" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7061,25 +7075,25 @@
         <v>20</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7093,7 +7107,7 @@
         <v>19</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E60" s="8">
         <v>45239</v>
@@ -7102,16 +7116,16 @@
         <v>45449</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7119,25 +7133,25 @@
         <v>20</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>1</v>
@@ -7154,7 +7168,7 @@
         <v>8</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E64" s="8">
         <v>45166</v>
@@ -7169,7 +7183,7 @@
         <v>2</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7183,7 +7197,7 @@
         <v>16</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E65" s="8">
         <v>45138</v>
@@ -7209,7 +7223,7 @@
         <v>16</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E66" s="8">
         <v>45177</v>
@@ -7235,7 +7249,7 @@
         <v>17</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E67" s="8">
         <v>45222</v>
@@ -7261,7 +7275,7 @@
         <v>17</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E68" s="8">
         <v>45174</v>
@@ -7287,7 +7301,7 @@
         <v>18</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E69" s="8">
         <v>45261</v>
@@ -7313,7 +7327,7 @@
         <v>19</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E70" s="8">
         <v>45174</v>
@@ -7339,7 +7353,7 @@
         <v>19</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E71" s="8">
         <v>45239</v>
@@ -7357,10 +7371,10 @@
     <row r="72" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="1:11" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7368,31 +7382,31 @@
         <v>20</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G74" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J74" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="K74" s="2" t="s">
         <v>1</v>
@@ -7409,7 +7423,7 @@
         <v>8</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E75" s="8">
         <v>45166</v>
@@ -7441,7 +7455,7 @@
         <v>8</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E76" s="8">
         <v>45118</v>
@@ -7473,7 +7487,7 @@
         <v>16</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E77" s="8">
         <v>45177</v>
@@ -7494,7 +7508,7 @@
         <v>54</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7508,7 +7522,7 @@
         <v>17</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E78" s="8">
         <v>45222</v>
@@ -7540,7 +7554,7 @@
         <v>17</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E79" s="8">
         <v>45174</v>
@@ -7572,7 +7586,7 @@
         <v>18</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E80" s="8">
         <v>45261</v>
@@ -7611,7 +7625,7 @@
     <row r="96" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="10">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -7628,11 +7642,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FDE18F-90A8-4CA6-8613-A02E9958E19E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FDE18F-90A8-4CA6-8613-A02E9958E19E}">
   <dimension ref="A1:V67"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7652,7 +7666,7 @@
     <col min="13" max="13" width="21" style="2" customWidth="1"/>
     <col min="14" max="14" width="16.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="18" style="2" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="2" customWidth="1"/>
     <col min="18" max="18" width="17.85546875" style="2" customWidth="1"/>
     <col min="19" max="19" width="24.42578125" style="2" customWidth="1"/>
@@ -7662,10 +7676,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -7674,7 +7688,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -7702,7 +7716,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>40</v>
@@ -7710,31 +7724,31 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E6" s="2">
         <v>10549000</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>43</v>
@@ -7743,25 +7757,25 @@
         <v>616004000</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="D8" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E8" s="2">
         <v>10549010</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7773,23 +7787,23 @@
         <v>616004070</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="D10" s="10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -7813,10 +7827,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -7824,10 +7838,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -7836,7 +7850,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -7865,7 +7879,7 @@
         <v>50</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>51</v>
@@ -7883,24 +7897,27 @@
         <v>55</v>
       </c>
       <c r="P17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="T17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="R17" s="2" t="s">
+      <c r="U17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="S17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B18" s="2">
         <v>2024</v>
@@ -7909,7 +7926,7 @@
         <v>616004070</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E18" s="8">
         <v>45110</v>
@@ -7918,7 +7935,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H18" s="8">
         <v>45138</v>
@@ -7927,7 +7944,7 @@
         <v>99</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K18" s="2">
         <v>4</v>
@@ -7936,33 +7953,36 @@
         <v>0</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O18" s="2">
         <v>10549000</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q18" s="19">
         <v>9</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="R18" s="2">
         <v>9</v>
       </c>
-      <c r="R18" s="2">
+      <c r="S18" s="2">
         <v>999</v>
       </c>
-      <c r="S18" s="2">
+      <c r="T18" s="2">
         <v>0</v>
       </c>
-      <c r="T18" s="2">
+      <c r="U18" s="2">
         <v>10549000</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B19" s="2">
         <v>2024</v>
@@ -7971,7 +7991,7 @@
         <v>616004070</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E19" s="8">
         <v>45174</v>
@@ -7980,7 +8000,7 @@
         <v>24</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H19" s="8">
         <v>45443</v>
@@ -7989,7 +8009,7 @@
         <v>40</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K19" s="2">
         <v>4</v>
@@ -7998,33 +8018,36 @@
         <v>0</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O19" s="2">
         <v>10549000</v>
       </c>
-      <c r="P19" s="2">
-        <v>390</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>390</v>
+      <c r="P19" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q19" s="19">
+        <v>39</v>
       </c>
       <c r="R19" s="2">
+        <v>39</v>
+      </c>
+      <c r="S19" s="2">
         <v>999</v>
       </c>
-      <c r="S19" s="2">
+      <c r="T19" s="2">
         <v>0</v>
       </c>
-      <c r="T19" s="2">
+      <c r="U19" s="2">
         <v>10549000</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B20" s="2">
         <v>2024</v>
@@ -8033,7 +8056,7 @@
         <v>616004070</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E20" s="8">
         <v>45181</v>
@@ -8042,7 +8065,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H20" s="8">
         <v>45212</v>
@@ -8051,7 +8074,7 @@
         <v>99</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K20" s="2">
         <v>2</v>
@@ -8060,33 +8083,36 @@
         <v>0</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O20" s="2">
         <v>10549000</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P20" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q20" s="19">
         <v>3</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="R20" s="2">
         <v>3</v>
       </c>
-      <c r="R20" s="2">
+      <c r="S20" s="2">
         <v>999</v>
       </c>
-      <c r="S20" s="2">
+      <c r="T20" s="2">
         <v>0</v>
       </c>
-      <c r="T20" s="2">
+      <c r="U20" s="2">
         <v>10549000</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B21" s="2">
         <v>2024</v>
@@ -8095,7 +8121,7 @@
         <v>616004070</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E21" s="8">
         <v>45215</v>
@@ -8104,7 +8130,7 @@
         <v>24</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H21" s="8">
         <v>45443</v>
@@ -8113,7 +8139,7 @@
         <v>40</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K21" s="2">
         <v>4</v>
@@ -8122,68 +8148,71 @@
         <v>0</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O21" s="2">
         <v>10549000</v>
       </c>
-      <c r="P21" s="2">
-        <v>390</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>390</v>
+      <c r="P21" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q21" s="19">
+        <v>39</v>
       </c>
       <c r="R21" s="2">
+        <v>39</v>
+      </c>
+      <c r="S21" s="2">
         <v>999</v>
       </c>
-      <c r="S21" s="2">
+      <c r="T21" s="2">
         <v>0</v>
       </c>
-      <c r="T21" s="2">
+      <c r="U21" s="2">
         <v>10549000</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:20" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:21" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B25" s="2">
         <v>616004070</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D25" s="2">
         <v>10549010</v>
@@ -8195,18 +8224,18 @@
         <v>45138</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B26" s="2">
         <v>616004070</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D26" s="2">
         <v>10549010</v>
@@ -8218,18 +8247,18 @@
         <v>45443</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B27" s="2">
         <v>616004070</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D27" s="2">
         <v>10549010</v>
@@ -8241,18 +8270,18 @@
         <v>45212</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B28" s="2">
         <v>616004070</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D28" s="2">
         <v>10549010</v>
@@ -8264,260 +8293,260 @@
         <v>45443</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H32" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J32" s="2" t="s">
+      <c r="M32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L32" s="2" t="s">
+      <c r="O32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="P32" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B33" s="2">
         <v>616004070</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G33" s="2">
         <v>11</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L33" s="8">
         <v>44258</v>
       </c>
       <c r="M33" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N33" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O33" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B34" s="12">
         <v>616004070</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G34" s="2">
         <v>11</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L34" s="8">
         <v>44258</v>
       </c>
       <c r="M34" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N34" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B35" s="2">
         <v>616004070</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G35" s="2">
         <v>11</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L35" s="8">
         <v>44642</v>
       </c>
       <c r="M35" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N35" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O35" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B36" s="12">
         <v>616004070</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G36" s="2">
         <v>11</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L36" s="8">
         <v>44642</v>
       </c>
       <c r="M36" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N36" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O36" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D39" s="10"/>
     </row>
@@ -8526,28 +8555,28 @@
         <v>20</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>37</v>
@@ -8555,16 +8584,16 @@
     </row>
     <row r="41" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B41">
         <v>616004070</v>
       </c>
       <c r="C41" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D41" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E41" s="8">
         <v>45108</v>
@@ -8573,9 +8602,9 @@
         <v>45138</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H41" s="2">
+        <v>151</v>
+      </c>
+      <c r="H41" s="19">
         <v>9</v>
       </c>
       <c r="I41" s="2">
@@ -8587,16 +8616,16 @@
     </row>
     <row r="42" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B42">
         <v>616004070</v>
       </c>
       <c r="C42" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D42" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E42" s="8">
         <v>45174</v>
@@ -8605,13 +8634,13 @@
         <v>45443</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H42" s="2">
-        <v>390</v>
+        <v>151</v>
+      </c>
+      <c r="H42" s="19">
+        <v>39</v>
       </c>
       <c r="I42" s="2">
-        <v>390</v>
+        <v>39</v>
       </c>
       <c r="J42" s="2">
         <v>999</v>
@@ -8619,16 +8648,16 @@
     </row>
     <row r="43" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B43">
         <v>616004070</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D43" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E43" s="8">
         <v>45181</v>
@@ -8637,9 +8666,9 @@
         <v>45212</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H43" s="2">
+        <v>151</v>
+      </c>
+      <c r="H43" s="19">
         <v>3</v>
       </c>
       <c r="I43" s="2">
@@ -8651,16 +8680,16 @@
     </row>
     <row r="44" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B44">
         <v>616004070</v>
       </c>
       <c r="C44" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D44" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E44" s="8">
         <v>45215</v>
@@ -8669,13 +8698,13 @@
         <v>45443</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H44" s="2">
-        <v>390</v>
+        <v>151</v>
+      </c>
+      <c r="H44" s="19">
+        <v>39</v>
       </c>
       <c r="I44" s="2">
-        <v>390</v>
+        <v>39</v>
       </c>
       <c r="J44" s="2">
         <v>999</v>
@@ -8687,7 +8716,7 @@
     </row>
     <row r="46" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D46" s="10"/>
     </row>
@@ -8696,45 +8725,45 @@
         <v>20</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B48" s="12">
         <v>616004070</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E48" s="8">
         <v>45110</v>
@@ -8757,16 +8786,16 @@
     </row>
     <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B49" s="12">
         <v>616004070</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D49" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E49" s="8">
         <v>45174</v>
@@ -8789,16 +8818,16 @@
     </row>
     <row r="50" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B50" s="12">
         <v>616004070</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D50" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E50" s="8">
         <v>45181</v>
@@ -8821,16 +8850,16 @@
     </row>
     <row r="51" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B51" s="12">
         <v>616004070</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D51" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E51" s="8">
         <v>45215</v>
@@ -8869,8 +8898,8 @@
     <row r="67" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <tableParts count="8">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -8878,7 +8907,6 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
-    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update some of the ancillary numbers in associated JP SEORA spreadsheet
</commit_message>
<xml_diff>
--- a/2024-25 MDE Ed-Fi Documentation/Joint_Powers_Vendor_Certification_Pattern_Data.xlsx
+++ b/2024-25 MDE Ed-Fi Documentation/Joint_Powers_Vendor_Certification_Pattern_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDolbow\.vscode\MDE-EdFi-Documentation\2024-25 MDE Ed-Fi Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AD47F1-EDF7-46BA-95FE-7513F152BD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5EDADB-5335-43B6-9B88-E7283A6A6EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B57C0786-A6AB-4FD4-B2B0-BA31B16F8519}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="178">
   <si>
     <t>Tab Name</t>
   </si>
@@ -713,6 +713,9 @@
   </si>
   <si>
     <t>The following data elements are informational only to demonstrate how associated records contain matching information with the SSA and SEORA records. Vendors will not be expected to create these separately.</t>
+  </si>
+  <si>
+    <t>No record required; zero will be the MARSS result</t>
   </si>
 </sst>
 </file>
@@ -922,7 +925,514 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -942,680 +1452,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2079,6 +1915,61 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -3364,6 +3255,44 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -3991,6 +3920,80 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -4581,10 +4584,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4606,193 +4605,193 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3CF0901-CC20-4EC6-A4BB-C588254B263D}" name="SSEPAs" displayName="SSEPAs" ref="A74:K80" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3CF0901-CC20-4EC6-A4BB-C588254B263D}" name="SSEPAs" displayName="SSEPAs" ref="A74:K80" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
   <autoFilter ref="A74:K80" xr:uid="{D3CF0901-CC20-4EC6-A4BB-C588254B263D}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EB40C147-90DE-48B5-8796-49E623DC4E7C}" name="Student" dataDxfId="110"/>
-    <tableColumn id="2" xr3:uid="{DBBEE278-F072-4B56-A6F8-DACC2223D596}" name="EdOrgReference SchoolID" dataDxfId="109"/>
-    <tableColumn id="3" xr3:uid="{C0A1BF68-1FB1-4480-B1C8-72DC3BFCAD22}" name="StudentUniqueId" dataDxfId="108"/>
-    <tableColumn id="4" xr3:uid="{24A13DCF-85C7-4DE6-8C3B-392BB7EC4C10}" name="ProgramType" dataDxfId="107"/>
-    <tableColumn id="5" xr3:uid="{D4EDE21F-3739-4CB6-BF74-3DFC09DC6F98}" name="BeginDate" dataDxfId="106"/>
-    <tableColumn id="6" xr3:uid="{6E1E1FFB-5065-4047-B6CE-377B73DA72C6}" name="EndDate" dataDxfId="105"/>
-    <tableColumn id="7" xr3:uid="{77B58A17-99F8-4B22-8571-A4BDF0118246}" name="DisabilityDescriptor" dataDxfId="104"/>
-    <tableColumn id="8" xr3:uid="{BC11DEE3-57F6-4A9E-B7B0-3C449D912E87}" name="OrderOfDisability" dataDxfId="103"/>
-    <tableColumn id="9" xr3:uid="{5D20C335-1671-4B9C-9E6C-CC5949CCA43E}" name="SpecialEducationSetting" dataDxfId="102"/>
-    <tableColumn id="10" xr3:uid="{4F4D10F4-5E8F-4AB4-81B1-7AB2D9F3AB81}" name="SpecialEducationServiceHours" dataDxfId="101"/>
-    <tableColumn id="11" xr3:uid="{D96C9E4B-D2F3-4C15-81D1-FA31E1D96253}" name="Notes" dataDxfId="100"/>
+    <tableColumn id="1" xr3:uid="{EB40C147-90DE-48B5-8796-49E623DC4E7C}" name="Student" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{DBBEE278-F072-4B56-A6F8-DACC2223D596}" name="EdOrgReference SchoolID" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{C0A1BF68-1FB1-4480-B1C8-72DC3BFCAD22}" name="StudentUniqueId" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{24A13DCF-85C7-4DE6-8C3B-392BB7EC4C10}" name="ProgramType" dataDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{D4EDE21F-3739-4CB6-BF74-3DFC09DC6F98}" name="BeginDate" dataDxfId="100"/>
+    <tableColumn id="6" xr3:uid="{6E1E1FFB-5065-4047-B6CE-377B73DA72C6}" name="EndDate" dataDxfId="99"/>
+    <tableColumn id="7" xr3:uid="{77B58A17-99F8-4B22-8571-A4BDF0118246}" name="DisabilityDescriptor" dataDxfId="98"/>
+    <tableColumn id="8" xr3:uid="{BC11DEE3-57F6-4A9E-B7B0-3C449D912E87}" name="OrderOfDisability" dataDxfId="97"/>
+    <tableColumn id="9" xr3:uid="{5D20C335-1671-4B9C-9E6C-CC5949CCA43E}" name="SpecialEducationSetting" dataDxfId="96"/>
+    <tableColumn id="10" xr3:uid="{4F4D10F4-5E8F-4AB4-81B1-7AB2D9F3AB81}" name="SpecialEducationServiceHours" dataDxfId="95"/>
+    <tableColumn id="11" xr3:uid="{D96C9E4B-D2F3-4C15-81D1-FA31E1D96253}" name="Notes" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{77FAAC26-2EEA-45D3-832C-0FF7AB0115F4}" name="SEORAs" displayName="SEORAs" ref="A33:G42" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{77FAAC26-2EEA-45D3-832C-0FF7AB0115F4}" name="SEORAs" displayName="SEORAs" ref="A33:G42" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <autoFilter ref="A33:G42" xr:uid="{77FAAC26-2EEA-45D3-832C-0FF7AB0115F4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:G42">
     <sortCondition ref="A34:A42"/>
     <sortCondition ref="E34:E42"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F05BB232-4DFB-4C6E-811E-2AF6253132F7}" name="Student" dataDxfId="97"/>
-    <tableColumn id="2" xr3:uid="{D4736AE3-CC59-41EA-BFA9-4EDC5622C627}" name="EdOrgReference SchoolID" dataDxfId="96"/>
-    <tableColumn id="3" xr3:uid="{344E6356-7C86-47AB-A9B5-171414F3EFAC}" name="StudentUniqueId" dataDxfId="95"/>
-    <tableColumn id="4" xr3:uid="{83C6D33C-247C-40CF-8422-32BAE1ACE4BA}" name="ReportingEdOrgReference SchoolID" dataDxfId="94"/>
-    <tableColumn id="5" xr3:uid="{16307EDC-78DB-420B-8467-0BAD8C2391FD}" name="BeginDate" dataDxfId="93"/>
-    <tableColumn id="6" xr3:uid="{2B61E709-93D0-41FC-BD9F-DA062C218CAC}" name="EndDate" dataDxfId="92"/>
-    <tableColumn id="7" xr3:uid="{46451781-17EF-44AB-BF2B-B4E3194F2583}" name="ResponsibiltyDescriptor" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{F05BB232-4DFB-4C6E-811E-2AF6253132F7}" name="Student" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{D4736AE3-CC59-41EA-BFA9-4EDC5622C627}" name="EdOrgReference SchoolID" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{344E6356-7C86-47AB-A9B5-171414F3EFAC}" name="StudentUniqueId" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{83C6D33C-247C-40CF-8422-32BAE1ACE4BA}" name="ReportingEdOrgReference SchoolID" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{16307EDC-78DB-420B-8467-0BAD8C2391FD}" name="BeginDate" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{2B61E709-93D0-41FC-BD9F-DA062C218CAC}" name="EndDate" dataDxfId="86"/>
+    <tableColumn id="7" xr3:uid="{46451781-17EF-44AB-BF2B-B4E3194F2583}" name="ResponsibiltyDescriptor" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{7A4D8A4E-B4D6-48EF-AE93-C41CB990E854}" name="Students13" displayName="Students13" ref="A5:B7" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{7A4D8A4E-B4D6-48EF-AE93-C41CB990E854}" name="Students13" displayName="Students13" ref="A5:B7" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
   <autoFilter ref="A5:B7" xr:uid="{E813628D-9E65-466B-AFAE-06C8ED720622}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{299B3E39-4326-4464-A557-F9C8B0EAC6B3}" name="Generic Name" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{062A82B9-5087-4506-AA8E-D7FE1B7660B4}" name="ID" dataDxfId="87"/>
+    <tableColumn id="1" xr3:uid="{299B3E39-4326-4464-A557-F9C8B0EAC6B3}" name="Generic Name" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{062A82B9-5087-4506-AA8E-D7FE1B7660B4}" name="ID" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{EE1C7247-5C59-4215-B4C5-0E8837A2BAF6}" name="Scenarios14" displayName="Scenarios14" ref="A12:C14" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{EE1C7247-5C59-4215-B4C5-0E8837A2BAF6}" name="Scenarios14" displayName="Scenarios14" ref="A12:C14" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
   <autoFilter ref="A12:C14" xr:uid="{6D6F743E-9CB8-4440-92A1-95FD6FFE6308}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{13C3256E-0CEE-41E5-85AC-724669B68AA2}" name="Scenario Identifier" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{F64DDA22-2EF1-4AB5-954C-9266230EF577}" name="Student" dataDxfId="83"/>
-    <tableColumn id="2" xr3:uid="{68C9BC3C-2995-4DCA-9514-BD8AA004ECC9}" name="Description" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{13C3256E-0CEE-41E5-85AC-724669B68AA2}" name="Scenario Identifier" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{F64DDA22-2EF1-4AB5-954C-9266230EF577}" name="Student" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{68C9BC3C-2995-4DCA-9514-BD8AA004ECC9}" name="Description" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{2C1A36F6-A443-478F-8632-701D4AC088EF}" name="SSAs15" displayName="SSAs15" ref="A17:U21" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{2C1A36F6-A443-478F-8632-701D4AC088EF}" name="SSAs15" displayName="SSAs15" ref="A17:U21" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <autoFilter ref="A17:U21" xr:uid="{85C15CF2-370D-42B8-85DC-039C7BB0A730}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:U21">
     <sortCondition ref="A18:A21"/>
     <sortCondition ref="E18:E21"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{77BD5FE2-7D29-4278-B63A-7A06AF887945}" name="Student" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{490DFC55-A99B-4943-BC4F-82BC3BAE0AB2}" name="SchoolYear" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{379DFE0A-3603-4E83-A069-1909CEEF2FBB}" name="SchoolReference SchoolID" dataDxfId="77"/>
-    <tableColumn id="4" xr3:uid="{954AA04A-3355-4EA1-8BF8-8B54D100FDED}" name="StudentUniqueId" dataDxfId="76"/>
-    <tableColumn id="5" xr3:uid="{9D720E08-5DCB-4550-8EC5-5DB73369328B}" name="EntryDate" dataDxfId="75"/>
-    <tableColumn id="6" xr3:uid="{248E7E85-0636-44F6-A9B7-3822FE17505C}" name="EntryType" dataDxfId="74"/>
-    <tableColumn id="7" xr3:uid="{8AB87614-E268-4037-B124-AD289B2038D3}" name="EntryGradeLevel" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{1E0CAC48-E2F8-4439-9A70-142378B29E11}" name="ExitWithdrawDate" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{8E363293-A545-4028-86AB-56D402E6B5DF}" name="ExitWithdrawType" dataDxfId="71"/>
-    <tableColumn id="10" xr3:uid="{643BDE56-57B7-44F0-9BF5-CBB7C61DE871}" name="CalendarReference" dataDxfId="70"/>
-    <tableColumn id="11" xr3:uid="{EA285CC7-0C07-4807-BAE0-C470FB431A3C}" name="SpecialEdEvalStatus" dataDxfId="69"/>
-    <tableColumn id="12" xr3:uid="{E4A73A11-17B0-47E2-9CA5-C2E7F1C386F4}" name="StateAidCategory" dataDxfId="68"/>
-    <tableColumn id="13" xr3:uid="{9479A754-4670-458F-9436-083720FA4EBA}" name="HomeboundService" dataDxfId="67"/>
-    <tableColumn id="14" xr3:uid="{C3053064-2B1E-4443-9801-38762BA25785}" name="SpecialPupil" dataDxfId="66"/>
-    <tableColumn id="15" xr3:uid="{6901B54C-5DCF-4EAB-9F58-2FE573BC7343}" name="ResidentLEAReference" dataDxfId="65"/>
-    <tableColumn id="21" xr3:uid="{E301F53A-9DEF-4B90-8299-0DED2B9E40A9}" name="MembershipAttendanceUnit" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{303CB387-33E4-4656-9582-02D45831B388}" name="Attendance" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{0705E415-91EB-4AF5-A47D-97AE74014A06}" name="Membership" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{9846E1C6-D5CD-422C-B9CF-54925AEC931C}" name="PercentEnrolled" dataDxfId="64"/>
-    <tableColumn id="19" xr3:uid="{7730A9C1-1558-4B94-AD1E-5AC7983CABDF}" name="TransportationCategory" dataDxfId="63"/>
-    <tableColumn id="20" xr3:uid="{0E474587-197B-49DB-A30A-C0D1EA91022A}" name="TransportationLEA" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{77BD5FE2-7D29-4278-B63A-7A06AF887945}" name="Student" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{490DFC55-A99B-4943-BC4F-82BC3BAE0AB2}" name="SchoolYear" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{379DFE0A-3603-4E83-A069-1909CEEF2FBB}" name="SchoolReference SchoolID" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{954AA04A-3355-4EA1-8BF8-8B54D100FDED}" name="StudentUniqueId" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{9D720E08-5DCB-4550-8EC5-5DB73369328B}" name="EntryDate" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{248E7E85-0636-44F6-A9B7-3822FE17505C}" name="EntryType" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{8AB87614-E268-4037-B124-AD289B2038D3}" name="EntryGradeLevel" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{1E0CAC48-E2F8-4439-9A70-142378B29E11}" name="ExitWithdrawDate" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{8E363293-A545-4028-86AB-56D402E6B5DF}" name="ExitWithdrawType" dataDxfId="65"/>
+    <tableColumn id="10" xr3:uid="{643BDE56-57B7-44F0-9BF5-CBB7C61DE871}" name="CalendarReference" dataDxfId="64"/>
+    <tableColumn id="11" xr3:uid="{EA285CC7-0C07-4807-BAE0-C470FB431A3C}" name="SpecialEdEvalStatus" dataDxfId="63"/>
+    <tableColumn id="12" xr3:uid="{E4A73A11-17B0-47E2-9CA5-C2E7F1C386F4}" name="StateAidCategory" dataDxfId="62"/>
+    <tableColumn id="13" xr3:uid="{9479A754-4670-458F-9436-083720FA4EBA}" name="HomeboundService" dataDxfId="61"/>
+    <tableColumn id="14" xr3:uid="{C3053064-2B1E-4443-9801-38762BA25785}" name="SpecialPupil" dataDxfId="60"/>
+    <tableColumn id="15" xr3:uid="{6901B54C-5DCF-4EAB-9F58-2FE573BC7343}" name="ResidentLEAReference" dataDxfId="59"/>
+    <tableColumn id="21" xr3:uid="{E301F53A-9DEF-4B90-8299-0DED2B9E40A9}" name="MembershipAttendanceUnit" dataDxfId="58"/>
+    <tableColumn id="16" xr3:uid="{303CB387-33E4-4656-9582-02D45831B388}" name="Attendance" dataDxfId="57"/>
+    <tableColumn id="17" xr3:uid="{0705E415-91EB-4AF5-A47D-97AE74014A06}" name="Membership" dataDxfId="56"/>
+    <tableColumn id="18" xr3:uid="{9846E1C6-D5CD-422C-B9CF-54925AEC931C}" name="PercentEnrolled" dataDxfId="55"/>
+    <tableColumn id="19" xr3:uid="{7730A9C1-1558-4B94-AD1E-5AC7983CABDF}" name="TransportationCategory" dataDxfId="54"/>
+    <tableColumn id="20" xr3:uid="{0E474587-197B-49DB-A30A-C0D1EA91022A}" name="TransportationLEA" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{933DABD0-7C61-4C14-8C2D-7ECEE4DC9E96}" name="SEOAs17" displayName="SEOAs17" ref="A32:P36" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{933DABD0-7C61-4C14-8C2D-7ECEE4DC9E96}" name="SEOAs17" displayName="SEOAs17" ref="A32:P36" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A32:P36" xr:uid="{6534E20D-6A8C-4341-99EF-71275021166D}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{25597A3C-3EA4-44A7-8097-CAAA149E535B}" name="Student" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{495C6C4D-ED0F-4012-849A-F9324268C84F}" name="EdOrgReference SchoolID" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{2044D62F-A399-4D84-97F0-D150BD43357E}" name="StudentUniqueId" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{3B06A6D0-BA8A-44C7-8D57-606D1972BE8E}" name="HispanicLatinoEthnicity" dataDxfId="56"/>
-    <tableColumn id="16" xr3:uid="{282E8BB4-A531-4F14-A37D-A14638E3CCF7}" name="AEO" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{09D96BB6-F2EC-4C98-8AFD-B2CC41648311}" name="Races" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{BE6E30C3-E2E6-498B-BBF6-247C69B37764}" name="Languages" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{3238F1D2-2EBD-4AD6-A8B8-88595FE99E58}" name="LanguageUse" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{43D10D56-20D4-43A4-A346-16EDC4B34B7D}" name="Sex" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{B05CAD9E-363B-4DB4-9216-197F9D00AD4F}" name="StudentCharacteristics" dataDxfId="50"/>
-    <tableColumn id="10" xr3:uid="{F09AAE73-1A66-4872-A5CB-940B5415F101}" name="StudentIdentificationCodes" dataDxfId="49"/>
-    <tableColumn id="11" xr3:uid="{DBBAA6D2-5572-4389-BF8B-9EEEE893F67A}" name="BirthDate" dataDxfId="48"/>
-    <tableColumn id="12" xr3:uid="{77E7AA90-037F-46F3-B330-251D01990E13}" name="FirstName" dataDxfId="47"/>
-    <tableColumn id="13" xr3:uid="{94BEEDD9-E26D-44A8-92B8-FBCC6FDC67DC}" name="MiddleName" dataDxfId="46"/>
-    <tableColumn id="14" xr3:uid="{06D259D8-D6F7-492D-8A6D-085312D3BF49}" name="LastSurname" dataDxfId="45"/>
-    <tableColumn id="15" xr3:uid="{DA761B55-5E97-4A0B-A331-050F6FCAE0A9}" name="OptOutIndicators" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{25597A3C-3EA4-44A7-8097-CAAA149E535B}" name="Student" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{495C6C4D-ED0F-4012-849A-F9324268C84F}" name="EdOrgReference SchoolID" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{2044D62F-A399-4D84-97F0-D150BD43357E}" name="StudentUniqueId" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{3B06A6D0-BA8A-44C7-8D57-606D1972BE8E}" name="HispanicLatinoEthnicity" dataDxfId="47"/>
+    <tableColumn id="16" xr3:uid="{282E8BB4-A531-4F14-A37D-A14638E3CCF7}" name="AEO" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{09D96BB6-F2EC-4C98-8AFD-B2CC41648311}" name="Races" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{BE6E30C3-E2E6-498B-BBF6-247C69B37764}" name="Languages" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{3238F1D2-2EBD-4AD6-A8B8-88595FE99E58}" name="LanguageUse" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{43D10D56-20D4-43A4-A346-16EDC4B34B7D}" name="Sex" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{B05CAD9E-363B-4DB4-9216-197F9D00AD4F}" name="StudentCharacteristics" dataDxfId="41"/>
+    <tableColumn id="10" xr3:uid="{F09AAE73-1A66-4872-A5CB-940B5415F101}" name="StudentIdentificationCodes" dataDxfId="40"/>
+    <tableColumn id="11" xr3:uid="{DBBAA6D2-5572-4389-BF8B-9EEEE893F67A}" name="BirthDate" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{77E7AA90-037F-46F3-B330-251D01990E13}" name="FirstName" dataDxfId="38"/>
+    <tableColumn id="13" xr3:uid="{94BEEDD9-E26D-44A8-92B8-FBCC6FDC67DC}" name="MiddleName" dataDxfId="37"/>
+    <tableColumn id="14" xr3:uid="{06D259D8-D6F7-492D-8A6D-085312D3BF49}" name="LastSurname" dataDxfId="36"/>
+    <tableColumn id="15" xr3:uid="{DA761B55-5E97-4A0B-A331-050F6FCAE0A9}" name="OptOutIndicators" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{56B15117-EF68-47B8-9FDE-F283DEBCB659}" name="SEEPAs18" displayName="SEEPAs18" ref="A40:J44" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{56B15117-EF68-47B8-9FDE-F283DEBCB659}" name="SEEPAs18" displayName="SEEPAs18" ref="A40:J44" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A40:J44" xr:uid="{26630F95-9A06-4446-8DD6-2558045FE47E}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{F9C602C3-335D-445D-8D80-DBCC2538FA70}" name="Student"/>
     <tableColumn id="2" xr3:uid="{E33091ED-F15B-4B45-8406-FD1032C809B3}" name="EdOrgReference SchoolID"/>
     <tableColumn id="3" xr3:uid="{7D335072-A366-47CA-BE62-1060CB51F345}" name="StudentUniqueId"/>
     <tableColumn id="4" xr3:uid="{4FBAD97B-6E30-4838-B1A0-1A5B601E0560}" name="ProgramType"/>
-    <tableColumn id="5" xr3:uid="{1F4A5107-6B4F-4593-BB24-DAFBF459CB86}" name="BeginDate" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{FFA7940C-750A-4FAF-A2EF-04ACEE4BB3B1}" name="EndDate" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{4CC98005-563F-47F2-9D0C-44B3C6F515A7}" name="MembershipAttendanceUnit" dataDxfId="39"/>
-    <tableColumn id="8" xr3:uid="{A6230774-C103-4ECF-AD18-30934165BED7}" name="Attendance" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{6EC83FCF-624B-4B71-BFDD-5C37C18FACC4}" name="Membership" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{31007089-EEE6-4945-ABEE-E51C34B6970B}" name="Percent Enrolled" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{1F4A5107-6B4F-4593-BB24-DAFBF459CB86}" name="BeginDate" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{FFA7940C-750A-4FAF-A2EF-04ACEE4BB3B1}" name="EndDate" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{4CC98005-563F-47F2-9D0C-44B3C6F515A7}" name="MembershipAttendanceUnit" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{A6230774-C103-4ECF-AD18-30934165BED7}" name="Attendance" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{6EC83FCF-624B-4B71-BFDD-5C37C18FACC4}" name="Membership" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{31007089-EEE6-4945-ABEE-E51C34B6970B}" name="Percent Enrolled" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{5692A297-79BF-4F9C-9126-9341754B759A}" name="SEORAs22" displayName="SEORAs22" ref="A24:G28" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{5692A297-79BF-4F9C-9126-9341754B759A}" name="SEORAs22" displayName="SEORAs22" ref="A24:G28" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A24:G28" xr:uid="{77FAAC26-2EEA-45D3-832C-0FF7AB0115F4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:G28">
     <sortCondition ref="A25:A28"/>
     <sortCondition ref="E25:E28"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{97BBDAA1-EEF4-4890-8CC6-F82A47B30DC3}" name="Student" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{E5BB4BAA-D5FE-494C-A12E-4E5CD1FEFE9B}" name="EdOrgReference SchoolID" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{A74DDED4-B75E-4848-97D9-1694DFE7B6C8}" name="StudentUniqueId" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{355E7FFD-F72E-4F56-BD11-829342E8EDCE}" name="ReportingEdOrgReference SchoolID" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{4EA8EC2D-F4E8-4AC9-8F4E-F658A2E86566}" name="BeginDate" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{6F2CC1BA-FBD7-4B28-A91B-22431AA0A9BC}" name="EndDate" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{5D24870A-BBBB-49F7-A22D-9BC354C82EE7}" name="ResponsibiltyDescriptor" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{97BBDAA1-EEF4-4890-8CC6-F82A47B30DC3}" name="Student" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{E5BB4BAA-D5FE-494C-A12E-4E5CD1FEFE9B}" name="EdOrgReference SchoolID" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{A74DDED4-B75E-4848-97D9-1694DFE7B6C8}" name="StudentUniqueId" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{355E7FFD-F72E-4F56-BD11-829342E8EDCE}" name="ReportingEdOrgReference SchoolID" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{4EA8EC2D-F4E8-4AC9-8F4E-F658A2E86566}" name="BeginDate" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{6F2CC1BA-FBD7-4B28-A91B-22431AA0A9BC}" name="EndDate" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{5D24870A-BBBB-49F7-A22D-9BC354C82EE7}" name="ResponsibiltyDescriptor" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{E2C8E32D-19BD-4526-BD62-D5BCA10CC455}" name="EdOrgIds23" displayName="EdOrgIds23" ref="D5:G10" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{E2C8E32D-19BD-4526-BD62-D5BCA10CC455}" name="EdOrgIds23" displayName="EdOrgIds23" ref="D5:G10" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="D5:G10" xr:uid="{E2C8E32D-19BD-4526-BD62-D5BCA10CC455}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FDD8D5C6-800F-4420-AE64-B80892DD5760}" name="Element" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{6E125EEB-7097-4769-8F32-19E6038EE69E}" name="Example ID" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{0922D666-F3DB-47C1-914F-77976F17A1B8}" name="Used In…For this Pattern" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{A977DE9F-420B-4361-B08C-A9FD32195551}" name="Reason" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{FDD8D5C6-800F-4420-AE64-B80892DD5760}" name="Element" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{6E125EEB-7097-4769-8F32-19E6038EE69E}" name="Example ID" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{0922D666-F3DB-47C1-914F-77976F17A1B8}" name="Used In…For this Pattern" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{A977DE9F-420B-4361-B08C-A9FD32195551}" name="Reason" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{8ECA3C70-6EF7-49D0-B684-3D141180DADB}" name="SSEPAs21" displayName="SSEPAs21" ref="A47:J51" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{8ECA3C70-6EF7-49D0-B684-3D141180DADB}" name="SSEPAs21" displayName="SSEPAs21" ref="A47:J51" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A47:J51" xr:uid="{D3CF0901-CC20-4EC6-A4BB-C588254B263D}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{E4DF4947-C3A2-484F-9044-02FFEC2121CC}" name="Student" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{7BAF099E-F389-4EF3-9391-CDA5FEC272D3}" name="EdOrgReference SchoolID" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{01FD7A9A-A19F-48A9-A931-041143D4B550}" name="StudentUniqueId" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{C5888552-F872-4891-82A6-71B6CEFFD6B1}" name="ProgramType" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{2B79307A-550E-4F01-8DD5-FE20AEC09EEF}" name="BeginDate" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{E3D74796-9820-4448-BF45-3877BF979345}" name="EndDate" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{20C673CA-FDFD-4929-A3EA-443A5768000E}" name="DisabilityDescriptor" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{B744BD5D-2FFC-4E93-9A56-B726A607287B}" name="OrderOfDisability" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{CA31B897-F85C-44E1-8EEE-B20CF3FE1A71}" name="SpecialEducationSetting" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{ACB63A65-6385-4A6E-BD2B-697EE91120C2}" name="SpecialEducationServiceHours" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{E4DF4947-C3A2-484F-9044-02FFEC2121CC}" name="Student" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{7BAF099E-F389-4EF3-9391-CDA5FEC272D3}" name="EdOrgReference SchoolID" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{01FD7A9A-A19F-48A9-A931-041143D4B550}" name="StudentUniqueId" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C5888552-F872-4891-82A6-71B6CEFFD6B1}" name="ProgramType" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{2B79307A-550E-4F01-8DD5-FE20AEC09EEF}" name="BeginDate" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{E3D74796-9820-4448-BF45-3877BF979345}" name="EndDate" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{20C673CA-FDFD-4929-A3EA-443A5768000E}" name="DisabilityDescriptor" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{B744BD5D-2FFC-4E93-9A56-B726A607287B}" name="OrderOfDisability" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{CA31B897-F85C-44E1-8EEE-B20CF3FE1A71}" name="SpecialEducationSetting" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{ACB63A65-6385-4A6E-BD2B-697EE91120C2}" name="SpecialEducationServiceHours" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4844,104 +4843,104 @@
     <tableColumn id="13" xr3:uid="{F73F852B-30BA-444D-8002-FB95BD31D484}" name="HomeboundService" dataDxfId="171"/>
     <tableColumn id="14" xr3:uid="{8CF7231E-E453-476C-80A5-696516A4E92E}" name="SpecialPupil" dataDxfId="170"/>
     <tableColumn id="15" xr3:uid="{54611861-C7B1-4E49-9D59-FA95E3AA1DDF}" name="ResidentLEAReference" dataDxfId="169"/>
-    <tableColumn id="21" xr3:uid="{438C1F18-E0A0-4604-A90C-3B2A4F7690BF}" name="MembershipAttendanceUnit" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{B00E0262-A73E-40C6-A2D1-5C01FEA1382D}" name="Attendance" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{4F7FD020-423E-4DAC-BACD-27A9147BB8D0}" name="Membership" dataDxfId="7"/>
-    <tableColumn id="18" xr3:uid="{9344241F-6C08-4119-A8BB-6C4A3BBD67D9}" name="PercentEnrolled" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{C050E003-D9FE-4A89-AD1F-B5B18A6BFAC3}" name="TransportationCategory" dataDxfId="168"/>
-    <tableColumn id="20" xr3:uid="{0692C374-1DB3-497F-8B1D-3728A0D56DE2}" name="TransportationLEA" dataDxfId="167"/>
+    <tableColumn id="21" xr3:uid="{438C1F18-E0A0-4604-A90C-3B2A4F7690BF}" name="MembershipAttendanceUnit" dataDxfId="168"/>
+    <tableColumn id="16" xr3:uid="{B00E0262-A73E-40C6-A2D1-5C01FEA1382D}" name="Attendance" dataDxfId="167"/>
+    <tableColumn id="17" xr3:uid="{4F7FD020-423E-4DAC-BACD-27A9147BB8D0}" name="Membership" dataDxfId="166"/>
+    <tableColumn id="18" xr3:uid="{9344241F-6C08-4119-A8BB-6C4A3BBD67D9}" name="PercentEnrolled" dataDxfId="165"/>
+    <tableColumn id="19" xr3:uid="{C050E003-D9FE-4A89-AD1F-B5B18A6BFAC3}" name="TransportationCategory" dataDxfId="164"/>
+    <tableColumn id="20" xr3:uid="{0692C374-1DB3-497F-8B1D-3728A0D56DE2}" name="TransportationLEA" dataDxfId="163"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F2BCDEC8-8E36-4C36-BE66-F0CF6D0EC644}" name="EdOrgIds" displayName="EdOrgIds" ref="D5:G10" totalsRowShown="0" headerRowDxfId="166" dataDxfId="165">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F2BCDEC8-8E36-4C36-BE66-F0CF6D0EC644}" name="EdOrgIds" displayName="EdOrgIds" ref="D5:G10" totalsRowShown="0" headerRowDxfId="162" dataDxfId="161">
   <autoFilter ref="D5:G10" xr:uid="{F2BCDEC8-8E36-4C36-BE66-F0CF6D0EC644}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8E85224E-E7A7-4FE6-8296-B643291CD515}" name="Element" dataDxfId="164"/>
-    <tableColumn id="2" xr3:uid="{82CD4B99-8DFA-476D-9708-9EE44D5FEEED}" name="Example ID" dataDxfId="163"/>
-    <tableColumn id="4" xr3:uid="{093AD196-E421-4873-8CF7-8828F582DC33}" name="Used In…For this Pattern" dataDxfId="162"/>
-    <tableColumn id="3" xr3:uid="{C1A37B0E-9E2F-4A1D-9EB8-4B6289B3EF5C}" name="Reason" dataDxfId="161"/>
+    <tableColumn id="1" xr3:uid="{8E85224E-E7A7-4FE6-8296-B643291CD515}" name="Element" dataDxfId="160"/>
+    <tableColumn id="2" xr3:uid="{82CD4B99-8DFA-476D-9708-9EE44D5FEEED}" name="Example ID" dataDxfId="159"/>
+    <tableColumn id="4" xr3:uid="{093AD196-E421-4873-8CF7-8828F582DC33}" name="Used In…For this Pattern" dataDxfId="158"/>
+    <tableColumn id="3" xr3:uid="{C1A37B0E-9E2F-4A1D-9EB8-4B6289B3EF5C}" name="Reason" dataDxfId="157"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6534E20D-6A8C-4341-99EF-71275021166D}" name="SEOAs" displayName="SEOAs" ref="A46:P51" totalsRowShown="0" headerRowDxfId="160" dataDxfId="159">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6534E20D-6A8C-4341-99EF-71275021166D}" name="SEOAs" displayName="SEOAs" ref="A46:P51" totalsRowShown="0" headerRowDxfId="156" dataDxfId="155">
   <autoFilter ref="A46:P51" xr:uid="{6534E20D-6A8C-4341-99EF-71275021166D}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{A4A3D2FA-EDEE-45D8-9A6E-286AEB0C5BAF}" name="Student" dataDxfId="158"/>
-    <tableColumn id="2" xr3:uid="{A4F12726-9355-482E-ACB5-BD97FDC71288}" name="EdOrgReference SchoolID" dataDxfId="157"/>
-    <tableColumn id="3" xr3:uid="{A43CAF59-3D92-41B2-8921-8D26AF385820}" name="StudentUniqueId" dataDxfId="156"/>
-    <tableColumn id="4" xr3:uid="{A1FC7C2A-8C5E-45CD-B0EC-3011A475BBF6}" name="HispanicLatinoEthnicity" dataDxfId="155"/>
-    <tableColumn id="16" xr3:uid="{7F867879-6DD8-4834-9F9C-F40372F0D69F}" name="AEO" dataDxfId="154"/>
-    <tableColumn id="5" xr3:uid="{88E4A252-66D7-440E-B436-F96D57455583}" name="Races" dataDxfId="153"/>
-    <tableColumn id="6" xr3:uid="{53538A8D-8B3E-45DC-A3BE-6E64C28691A4}" name="Languages" dataDxfId="152"/>
-    <tableColumn id="7" xr3:uid="{D23E5EE2-E77E-457E-8165-58CE95E357EA}" name="LanguageUse" dataDxfId="151"/>
-    <tableColumn id="8" xr3:uid="{8679C1C7-0B37-4284-BF26-B514074CA756}" name="Sex" dataDxfId="150"/>
-    <tableColumn id="9" xr3:uid="{2A8D3774-405C-4EC5-A4E9-FE6BCC9ADE70}" name="StudentCharacteristics" dataDxfId="149"/>
-    <tableColumn id="10" xr3:uid="{542FCA80-189D-4AEE-855C-31A39E5EB85B}" name="StudentIdentificationCodes" dataDxfId="148"/>
-    <tableColumn id="11" xr3:uid="{3CB29F9B-A7A6-4565-B260-2906AF84129F}" name="BirthDate" dataDxfId="147"/>
-    <tableColumn id="12" xr3:uid="{080B3624-FBF4-45A9-A4CC-0698348072EE}" name="FirstName" dataDxfId="146"/>
-    <tableColumn id="13" xr3:uid="{F42D074E-6F35-489F-8757-9F408445D91C}" name="MiddleName" dataDxfId="145"/>
-    <tableColumn id="14" xr3:uid="{B839DA8B-9F76-46DA-9A57-B55DB230E6CA}" name="LastSurname" dataDxfId="144"/>
-    <tableColumn id="15" xr3:uid="{D6DFBB36-E469-4FB9-A50A-3ED2BDAD3CC4}" name="OptOutIndicators" dataDxfId="143"/>
+    <tableColumn id="1" xr3:uid="{A4A3D2FA-EDEE-45D8-9A6E-286AEB0C5BAF}" name="Student" dataDxfId="154"/>
+    <tableColumn id="2" xr3:uid="{A4F12726-9355-482E-ACB5-BD97FDC71288}" name="EdOrgReference SchoolID" dataDxfId="153"/>
+    <tableColumn id="3" xr3:uid="{A43CAF59-3D92-41B2-8921-8D26AF385820}" name="StudentUniqueId" dataDxfId="152"/>
+    <tableColumn id="4" xr3:uid="{A1FC7C2A-8C5E-45CD-B0EC-3011A475BBF6}" name="HispanicLatinoEthnicity" dataDxfId="151"/>
+    <tableColumn id="16" xr3:uid="{7F867879-6DD8-4834-9F9C-F40372F0D69F}" name="AEO" dataDxfId="150"/>
+    <tableColumn id="5" xr3:uid="{88E4A252-66D7-440E-B436-F96D57455583}" name="Races" dataDxfId="149"/>
+    <tableColumn id="6" xr3:uid="{53538A8D-8B3E-45DC-A3BE-6E64C28691A4}" name="Languages" dataDxfId="148"/>
+    <tableColumn id="7" xr3:uid="{D23E5EE2-E77E-457E-8165-58CE95E357EA}" name="LanguageUse" dataDxfId="147"/>
+    <tableColumn id="8" xr3:uid="{8679C1C7-0B37-4284-BF26-B514074CA756}" name="Sex" dataDxfId="146"/>
+    <tableColumn id="9" xr3:uid="{2A8D3774-405C-4EC5-A4E9-FE6BCC9ADE70}" name="StudentCharacteristics" dataDxfId="145"/>
+    <tableColumn id="10" xr3:uid="{542FCA80-189D-4AEE-855C-31A39E5EB85B}" name="StudentIdentificationCodes" dataDxfId="144"/>
+    <tableColumn id="11" xr3:uid="{3CB29F9B-A7A6-4565-B260-2906AF84129F}" name="BirthDate" dataDxfId="143"/>
+    <tableColumn id="12" xr3:uid="{080B3624-FBF4-45A9-A4CC-0698348072EE}" name="FirstName" dataDxfId="142"/>
+    <tableColumn id="13" xr3:uid="{F42D074E-6F35-489F-8757-9F408445D91C}" name="MiddleName" dataDxfId="141"/>
+    <tableColumn id="14" xr3:uid="{B839DA8B-9F76-46DA-9A57-B55DB230E6CA}" name="LastSurname" dataDxfId="140"/>
+    <tableColumn id="15" xr3:uid="{D6DFBB36-E469-4FB9-A50A-3ED2BDAD3CC4}" name="OptOutIndicators" dataDxfId="139"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{26630F95-9A06-4446-8DD6-2558045FE47E}" name="SEEPAs" displayName="SEEPAs" ref="A55:J56" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{26630F95-9A06-4446-8DD6-2558045FE47E}" name="SEEPAs" displayName="SEEPAs" ref="A55:J56" totalsRowShown="0" headerRowDxfId="138" dataDxfId="137">
   <autoFilter ref="A55:J56" xr:uid="{26630F95-9A06-4446-8DD6-2558045FE47E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F4C6ABD2-814B-4123-8E5A-62079CA8844E}" name="Student" dataDxfId="140"/>
-    <tableColumn id="2" xr3:uid="{B47E9466-2F59-40DC-BC6B-CCAFF687EA9F}" name="EdOrgReference SchoolID" dataDxfId="139"/>
-    <tableColumn id="3" xr3:uid="{13703732-AC7D-4B9C-AE0A-35BCC984E0F3}" name="StudentUniqueId" dataDxfId="138"/>
-    <tableColumn id="4" xr3:uid="{53FFB636-DB86-49B1-AA7D-9F15D7AEBACE}" name="ProgramType" dataDxfId="137"/>
-    <tableColumn id="5" xr3:uid="{8F49C286-C71C-4CAB-B47B-68D3411F7ECE}" name="BeginDate" dataDxfId="136"/>
-    <tableColumn id="6" xr3:uid="{2F2AFF46-9F5C-4FE0-B496-DF6C18DE9E8A}" name="EndDate" dataDxfId="135"/>
-    <tableColumn id="7" xr3:uid="{1C8C41F3-0DAB-49F7-B6A8-64F735833315}" name="MembershipAttendanceUnit" dataDxfId="134"/>
-    <tableColumn id="8" xr3:uid="{32BDBBC3-62E9-4D26-99AF-88573C5F627F}" name="Attendance" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{C723C480-F019-464D-9822-41DCD668AC80}" name="Membership" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{1067938B-0918-498E-9584-5C9C2E812DE2}" name="Percent Enrolled" dataDxfId="133"/>
+    <tableColumn id="1" xr3:uid="{F4C6ABD2-814B-4123-8E5A-62079CA8844E}" name="Student" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{B47E9466-2F59-40DC-BC6B-CCAFF687EA9F}" name="EdOrgReference SchoolID" dataDxfId="135"/>
+    <tableColumn id="3" xr3:uid="{13703732-AC7D-4B9C-AE0A-35BCC984E0F3}" name="StudentUniqueId" dataDxfId="134"/>
+    <tableColumn id="4" xr3:uid="{53FFB636-DB86-49B1-AA7D-9F15D7AEBACE}" name="ProgramType" dataDxfId="133"/>
+    <tableColumn id="5" xr3:uid="{8F49C286-C71C-4CAB-B47B-68D3411F7ECE}" name="BeginDate" dataDxfId="132"/>
+    <tableColumn id="6" xr3:uid="{2F2AFF46-9F5C-4FE0-B496-DF6C18DE9E8A}" name="EndDate" dataDxfId="131"/>
+    <tableColumn id="7" xr3:uid="{1C8C41F3-0DAB-49F7-B6A8-64F735833315}" name="MembershipAttendanceUnit" dataDxfId="130"/>
+    <tableColumn id="8" xr3:uid="{32BDBBC3-62E9-4D26-99AF-88573C5F627F}" name="Attendance" dataDxfId="129"/>
+    <tableColumn id="9" xr3:uid="{C723C480-F019-464D-9822-41DCD668AC80}" name="Membership" dataDxfId="128"/>
+    <tableColumn id="10" xr3:uid="{1067938B-0918-498E-9584-5C9C2E812DE2}" name="Percent Enrolled" dataDxfId="127"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CE1A2133-3BCA-425D-8B3A-B8B9EC1563A6}" name="SHPAs" displayName="SHPAs" ref="A59:H60" totalsRowShown="0" headerRowDxfId="132">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CE1A2133-3BCA-425D-8B3A-B8B9EC1563A6}" name="SHPAs" displayName="SHPAs" ref="A59:H60" totalsRowShown="0" headerRowDxfId="126">
   <autoFilter ref="A59:H60" xr:uid="{CE1A2133-3BCA-425D-8B3A-B8B9EC1563A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{04F78B13-55C3-43E3-95AF-59AF667F7DFB}" name="Student" dataDxfId="131"/>
-    <tableColumn id="2" xr3:uid="{7AE0FA1D-F422-466D-BE2F-56A5145E58EF}" name="EdOrgReference SchoolID" dataDxfId="130"/>
-    <tableColumn id="3" xr3:uid="{D8E0F478-4BB1-43DC-92E9-40EDF28DCFF2}" name="StudentUniqueId" dataDxfId="129"/>
-    <tableColumn id="4" xr3:uid="{ABC62F79-6030-4B33-A9EF-ABF1DC62BE62}" name="ProgramType" dataDxfId="128"/>
-    <tableColumn id="5" xr3:uid="{0634D05E-EB78-4F6C-A8B2-10BC6D46DB5C}" name="BeginDate" dataDxfId="127"/>
-    <tableColumn id="6" xr3:uid="{44F548B9-8217-43E0-B167-4C6D4A84F092}" name="EndDate" dataDxfId="126"/>
-    <tableColumn id="7" xr3:uid="{30CFA4E9-CEE8-4738-B52D-510A0602B8D4}" name="PrimaryNighttimeResidence" dataDxfId="125"/>
-    <tableColumn id="8" xr3:uid="{908C03ED-48BA-4124-B77C-EB692F9777B2}" name="Unaccompanied" dataDxfId="124"/>
+    <tableColumn id="1" xr3:uid="{04F78B13-55C3-43E3-95AF-59AF667F7DFB}" name="Student" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{7AE0FA1D-F422-466D-BE2F-56A5145E58EF}" name="EdOrgReference SchoolID" dataDxfId="124"/>
+    <tableColumn id="3" xr3:uid="{D8E0F478-4BB1-43DC-92E9-40EDF28DCFF2}" name="StudentUniqueId" dataDxfId="123"/>
+    <tableColumn id="4" xr3:uid="{ABC62F79-6030-4B33-A9EF-ABF1DC62BE62}" name="ProgramType" dataDxfId="122"/>
+    <tableColumn id="5" xr3:uid="{0634D05E-EB78-4F6C-A8B2-10BC6D46DB5C}" name="BeginDate" dataDxfId="121"/>
+    <tableColumn id="6" xr3:uid="{44F548B9-8217-43E0-B167-4C6D4A84F092}" name="EndDate" dataDxfId="120"/>
+    <tableColumn id="7" xr3:uid="{30CFA4E9-CEE8-4738-B52D-510A0602B8D4}" name="PrimaryNighttimeResidence" dataDxfId="119"/>
+    <tableColumn id="8" xr3:uid="{908C03ED-48BA-4124-B77C-EB692F9777B2}" name="Unaccompanied" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D73DF4A3-0B69-423F-AE1A-12C79E70A91B}" name="SSFSPAs" displayName="SSFSPAs" ref="A63:I71" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D73DF4A3-0B69-423F-AE1A-12C79E70A91B}" name="SSFSPAs" displayName="SSFSPAs" ref="A63:I71" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
   <autoFilter ref="A63:I71" xr:uid="{D73DF4A3-0B69-423F-AE1A-12C79E70A91B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6726B54E-590F-4630-B499-DF209BD6B268}" name="Student" dataDxfId="121"/>
-    <tableColumn id="2" xr3:uid="{A04B0A75-89FE-461C-9F22-40FC8BBE7988}" name="EdOrgReference SchoolID" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{7C3FAEFA-56A7-41F9-8E6F-CA76242BEEE2}" name="StudentUniqueId" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{2FF748BD-2F0E-4FF7-8B34-0F37E874D63E}" name="ProgramType" dataDxfId="118"/>
-    <tableColumn id="5" xr3:uid="{5E2E2E38-8BB5-4561-BD41-B7C7C5644445}" name="BeginDate" dataDxfId="117"/>
-    <tableColumn id="6" xr3:uid="{C597EBBD-6F81-400F-AAA1-7E35A1A81904}" name="EndDate" dataDxfId="116"/>
-    <tableColumn id="7" xr3:uid="{5AF3867E-7461-42FB-B199-114ABC8D724C}" name="Direct Certification" dataDxfId="115"/>
-    <tableColumn id="8" xr3:uid="{60A3ECAD-2AF3-45D7-ACE7-7F63BCAE08DC}" name="School Food Service Program Service" dataDxfId="114"/>
-    <tableColumn id="9" xr3:uid="{725AB688-A37C-47F1-BCBD-ED89B3141417}" name="Notes" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{6726B54E-590F-4630-B499-DF209BD6B268}" name="Student" dataDxfId="115"/>
+    <tableColumn id="2" xr3:uid="{A04B0A75-89FE-461C-9F22-40FC8BBE7988}" name="EdOrgReference SchoolID" dataDxfId="114"/>
+    <tableColumn id="3" xr3:uid="{7C3FAEFA-56A7-41F9-8E6F-CA76242BEEE2}" name="StudentUniqueId" dataDxfId="113"/>
+    <tableColumn id="4" xr3:uid="{2FF748BD-2F0E-4FF7-8B34-0F37E874D63E}" name="ProgramType" dataDxfId="112"/>
+    <tableColumn id="5" xr3:uid="{5E2E2E38-8BB5-4561-BD41-B7C7C5644445}" name="BeginDate" dataDxfId="111"/>
+    <tableColumn id="6" xr3:uid="{C597EBBD-6F81-400F-AAA1-7E35A1A81904}" name="EndDate" dataDxfId="110"/>
+    <tableColumn id="7" xr3:uid="{5AF3867E-7461-42FB-B199-114ABC8D724C}" name="Direct Certification" dataDxfId="109"/>
+    <tableColumn id="8" xr3:uid="{60A3ECAD-2AF3-45D7-ACE7-7F63BCAE08DC}" name="School Food Service Program Service" dataDxfId="108"/>
+    <tableColumn id="9" xr3:uid="{725AB688-A37C-47F1-BCBD-ED89B3141417}" name="Notes" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5266,7 +5265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA5FF19-54A6-4517-A0A6-3EE6F2194B71}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -5528,8 +5527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136FD443-4433-4AA8-9391-F8565D648BB7}">
   <dimension ref="A1:W96"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,6 +7262,9 @@
       <c r="H67" s="2">
         <v>0</v>
       </c>
+      <c r="I67" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="68" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
@@ -7289,6 +7291,9 @@
       <c r="H68" s="2">
         <v>0</v>
       </c>
+      <c r="I68" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="69" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
@@ -7314,6 +7319,9 @@
       </c>
       <c r="H69" s="2">
         <v>0</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7441,7 +7449,7 @@
         <v>3</v>
       </c>
       <c r="J75" s="2">
-        <v>11228</v>
+        <v>1122.8</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7473,7 +7481,7 @@
         <v>3</v>
       </c>
       <c r="J76" s="2">
-        <v>525</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7505,7 +7513,7 @@
         <v>1</v>
       </c>
       <c r="J77" s="2">
-        <v>54</v>
+        <v>5.4</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>103</v>
@@ -7540,7 +7548,7 @@
         <v>1</v>
       </c>
       <c r="J78" s="2">
-        <v>5463</v>
+        <v>546.29999999999995</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7571,8 +7579,8 @@
       <c r="I79" s="2">
         <v>1</v>
       </c>
-      <c r="J79" s="2">
-        <v>500</v>
+      <c r="J79" s="19">
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7604,7 +7612,7 @@
         <v>41</v>
       </c>
       <c r="J80" s="2">
-        <v>2592</v>
+        <v>259.2</v>
       </c>
     </row>
     <row r="81" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -7645,7 +7653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FDE18F-90A8-4CA6-8613-A02E9958E19E}">
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>

</xml_diff>